<commit_message>
ainda no menu de emblemas
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\root\forMyGames\Jogos\Rectangle Knight\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504FEF8D-446B-402E-8D9D-ED23A2AFC227}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="listaDeTarefasComEstimativas" sheetId="2" r:id="rId1"/>
@@ -17,12 +18,12 @@
     <sheet name="timeLineDoProjeto" sheetId="3" r:id="rId3"/>
     <sheet name="horasTrabalhadas" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="120">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -375,13 +376,19 @@
     <t>10h-11h30min</t>
   </si>
   <si>
-    <t>3h30min</t>
+    <t>15h30 - 17h</t>
+  </si>
+  <si>
+    <t>12h30min-13h30min</t>
+  </si>
+  <si>
+    <t>18h15min-20h45min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\ \ mmm\ \ yyyy"/>
   </numFmts>
@@ -675,7 +682,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" applyNumberFormat="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -707,9 +714,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -744,6 +748,21 @@
     <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="40% - Ênfase3" xfId="4" builtinId="39"/>
@@ -752,7 +771,7 @@
     <cellStyle name="Nota" xfId="5" builtinId="10"/>
     <cellStyle name="Saída" xfId="1" builtinId="21"/>
     <cellStyle name="Título 4" xfId="2" builtinId="19"/>
-    <cellStyle name="verdinhoDaTabela" xfId="6"/>
+    <cellStyle name="verdinhoDaTabela" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -851,6 +870,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -886,6 +922,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1061,11 +1114,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,7 +1563,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B4:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1869,11 +1922,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:DT15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,75 +1938,75 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:124" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="19"/>
-      <c r="AI3" s="19"/>
-      <c r="AJ3" s="21" t="s">
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="34"/>
+      <c r="W3" s="34"/>
+      <c r="X3" s="34"/>
+      <c r="Y3" s="34"/>
+      <c r="Z3" s="34"/>
+      <c r="AA3" s="34"/>
+      <c r="AB3" s="34"/>
+      <c r="AC3" s="34"/>
+      <c r="AD3" s="34"/>
+      <c r="AE3" s="34"/>
+      <c r="AF3" s="34"/>
+      <c r="AG3" s="34"/>
+      <c r="AH3" s="34"/>
+      <c r="AI3" s="35"/>
+      <c r="AJ3" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="AK3" s="21"/>
-      <c r="AL3" s="21"/>
-      <c r="AM3" s="21"/>
-      <c r="AN3" s="21"/>
-      <c r="AO3" s="21"/>
-      <c r="AP3" s="21"/>
-      <c r="AQ3" s="21"/>
-      <c r="AR3" s="21"/>
-      <c r="AS3" s="21"/>
-      <c r="AT3" s="21"/>
-      <c r="AU3" s="21"/>
-      <c r="AV3" s="21"/>
-      <c r="AW3" s="21"/>
-      <c r="AX3" s="21"/>
-      <c r="AY3" s="21"/>
-      <c r="AZ3" s="21"/>
-      <c r="BA3" s="21"/>
-      <c r="BB3" s="21"/>
-      <c r="BC3" s="21"/>
-      <c r="BD3" s="21"/>
-      <c r="BE3" s="21"/>
-      <c r="BF3" s="21"/>
-      <c r="BG3" s="21"/>
-      <c r="BH3" s="21"/>
-      <c r="BI3" s="21"/>
-      <c r="BJ3" s="21"/>
-      <c r="BK3" s="21"/>
-      <c r="BL3" s="21"/>
-      <c r="BM3" s="21"/>
+      <c r="AK3" s="20"/>
+      <c r="AL3" s="20"/>
+      <c r="AM3" s="20"/>
+      <c r="AN3" s="20"/>
+      <c r="AO3" s="20"/>
+      <c r="AP3" s="20"/>
+      <c r="AQ3" s="20"/>
+      <c r="AR3" s="20"/>
+      <c r="AS3" s="20"/>
+      <c r="AT3" s="20"/>
+      <c r="AU3" s="20"/>
+      <c r="AV3" s="20"/>
+      <c r="AW3" s="20"/>
+      <c r="AX3" s="20"/>
+      <c r="AY3" s="20"/>
+      <c r="AZ3" s="20"/>
+      <c r="BA3" s="20"/>
+      <c r="BB3" s="20"/>
+      <c r="BC3" s="20"/>
+      <c r="BD3" s="20"/>
+      <c r="BE3" s="20"/>
+      <c r="BF3" s="20"/>
+      <c r="BG3" s="20"/>
+      <c r="BH3" s="20"/>
+      <c r="BI3" s="20"/>
+      <c r="BJ3" s="20"/>
+      <c r="BK3" s="20"/>
+      <c r="BL3" s="20"/>
+      <c r="BM3" s="20"/>
       <c r="BN3" s="19" t="s">
         <v>61</v>
       </c>
@@ -2460,6 +2515,8 @@
       </c>
       <c r="R15" s="11"/>
       <c r="S15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2547,40 +2604,39 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Y39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A3:AD39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <pane xSplit="3" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="10" width="21.85546875" customWidth="1"/>
-    <col min="11" max="19" width="4.42578125" customWidth="1"/>
-    <col min="20" max="23" width="3.85546875" customWidth="1"/>
-    <col min="24" max="25" width="4.85546875" customWidth="1"/>
+    <col min="4" max="29" width="18.85546875" customWidth="1"/>
+    <col min="30" max="30" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <v>43523</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="22">
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="21">
         <v>43524</v>
       </c>
-      <c r="H4" s="22"/>
+      <c r="H4" s="21"/>
       <c r="I4" s="7">
         <v>43525</v>
       </c>
@@ -2590,20 +2646,20 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="29">
+      <c r="L4" s="28">
         <v>43530</v>
       </c>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="22">
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="21">
         <v>43531</v>
       </c>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22">
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21">
         <v>43532</v>
       </c>
-      <c r="S4" s="22"/>
+      <c r="S4" s="21"/>
       <c r="T4" s="7">
         <v>43533</v>
       </c>
@@ -2622,8 +2678,17 @@
       <c r="Y4" s="7">
         <v>43539</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z4" s="21">
+        <v>43542</v>
+      </c>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="21">
+        <v>43543</v>
+      </c>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="21"/>
+    </row>
+    <row r="5" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2643,7 +2708,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2657,7 +2722,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2671,7 +2736,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2685,41 +2750,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="26" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="J10" s="28"/>
-    </row>
-    <row r="11" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="24"/>
+      <c r="J10" s="27"/>
+    </row>
+    <row r="11" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="J11" s="28"/>
-    </row>
-    <row r="12" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="25"/>
+      <c r="J11" s="27"/>
+    </row>
+    <row r="12" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2733,7 +2798,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2765,7 +2830,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2773,7 +2838,7 @@
         <v>72</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="X14" s="18" t="s">
         <v>115</v>
@@ -2781,8 +2846,23 @@
       <c r="Y14" s="11" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z14" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA14" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB14" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC14" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD14" s="17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -2814,7 +2894,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -2916,14 +2996,16 @@
     <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="Z4:AA4"/>
     <mergeCell ref="R4:S4"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="L4:O4"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A26">
     <cfRule type="colorScale" priority="8">

</xml_diff>

<commit_message>
terminado menu de pause
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\root\forMyGames\Jogos\Rectangle Knight\Assets\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{504FEF8D-446B-402E-8D9D-ED23A2AFC227}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="listaDeTarefasComEstimativas" sheetId="2" r:id="rId1"/>
     <sheet name="tarefas copiadas do cara" sheetId="1" r:id="rId2"/>
     <sheet name="timeLineDoProjeto" sheetId="3" r:id="rId3"/>
     <sheet name="horasTrabalhadas" sheetId="4" r:id="rId4"/>
+    <sheet name="mercado" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="162">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -383,16 +378,142 @@
   </si>
   <si>
     <t>18h15min-20h45min</t>
+  </si>
+  <si>
+    <t>12h30min - 13h30min</t>
+  </si>
+  <si>
+    <t>12h30min</t>
+  </si>
+  <si>
+    <t>Jogos Testados</t>
+  </si>
+  <si>
+    <t>produtor</t>
+  </si>
+  <si>
+    <t>Dungeon Vs Dungeon</t>
+  </si>
+  <si>
+    <t>Playone</t>
+  </si>
+  <si>
+    <t>Notas Google Play</t>
+  </si>
+  <si>
+    <t>Impressões de Jogabilidade</t>
+  </si>
+  <si>
+    <t>A jogabiliade é lenta com pulos baixos, como a maioria dos jogos de android a jogabilidade é bastante imprecisa</t>
+  </si>
+  <si>
+    <t>qualidade</t>
+  </si>
+  <si>
+    <t>A inserção de propagandas como armadilhas e para obtenção de itens foi bastante interessante. A historia a pesar de extremamente cliche cativa. O balanceamento do jogo estava bom até o segundo chefe.</t>
+  </si>
+  <si>
+    <t>Defeitos</t>
+  </si>
+  <si>
+    <t>Desisti do jogo no segundo chefe pois não tinha a menor chance de vence-lo. Talvez tenha se devido a eu ter evitado baus de propaganda que ofereciam moedas de updates, essas moedas devem ter feito extrema falta para enfrentar esse chefe</t>
+  </si>
+  <si>
+    <t>Tiny Dangerous Dungeons</t>
+  </si>
+  <si>
+    <t>Adventure Islands</t>
+  </si>
+  <si>
+    <t>A jogabilidade é boa e cumpre bem o seu papel, a escolha de design de evitar combates dibrou a impressisão da jogabilidade com botões na tela</t>
+  </si>
+  <si>
+    <t>Mapa claro, com conexões bem explicitas, sistema de updates simples e de fácil compreenção</t>
+  </si>
+  <si>
+    <t>O botão de pulo é o mesmo de ação ocasionando interações indesejadas. Hitbox as vezes nos confunde</t>
+  </si>
+  <si>
+    <t>baixado</t>
+  </si>
+  <si>
+    <t>Twisted Tales : Night Night Scarlett (não lançado)</t>
+  </si>
+  <si>
+    <t>Very Long Call</t>
+  </si>
+  <si>
+    <t>N/H</t>
+  </si>
+  <si>
+    <t>Os botões na tela responderam bem nos momentos em que eu testei. O pulo é alto e interessante, peca um ppouco na visibilidade do cenario</t>
+  </si>
+  <si>
+    <t>A resposta dos comandos é boa, o ataque é interessante, o pulo é alto com mais sensação de mobilidade, ideias padrões de coletáveis implementadas de maneira tradicional</t>
+  </si>
+  <si>
+    <t>inimigos em fases iniciais com comportamentos agressivos de mais. Level design não deixa claro o que pisavel ou não e isso é usado para criar armadilhas para o jogador. A quatidade de vida em comparação com o nivel de desafio inicial parece desequilibrada.</t>
+  </si>
+  <si>
+    <t>+1.000</t>
+  </si>
+  <si>
+    <t>+100.000</t>
+  </si>
+  <si>
+    <t>Tales of a Lost Mine (não lançado)</t>
+  </si>
+  <si>
+    <t>Fire Slime</t>
+  </si>
+  <si>
+    <t>Os botões na tela não são muito exigidos mas respondem bem. O botão de ação acabou me confundinco pois o visual do jogo era parecido com o que a ação era o pulo.</t>
+  </si>
+  <si>
+    <t>Movimentação lenta, pulo baixo e lento, problemas de design: o visual do jogo não deixa claro quando vai tomar dano, inimigos muito grandes para pular por eles sem tomar dano, design de armadilhas injusto</t>
+  </si>
+  <si>
+    <t>Não tem caracteristicas de metroidvania</t>
+  </si>
+  <si>
+    <t>Os defeitos de design me irritaram</t>
+  </si>
+  <si>
+    <t>Fin &amp; Ancient Mystery: platformer adventure</t>
+  </si>
+  <si>
+    <t>fenechGames</t>
+  </si>
+  <si>
+    <t>Meu celular deu Lag nesse jogo isso deve ter prejudicado a experiencia. Os comandos também sofreram atraso e os pulos ficaram completamente impressisos, claro que tudo isso deve ser devido ao Lag</t>
+  </si>
+  <si>
+    <t>Graficos com qualidade supeior aos outros jogos testados. Textos de tutorial bastante explicativos</t>
+  </si>
+  <si>
+    <t>Plataformas temporizadas demoradas de mais. Level Design não muito claro (portas são abertas em algum lugar do mapa com um lerp de camera que ocorre rapido demais). Inimigos causam dano não evitável (talvez por Lag). Dano de espinhos também dificil de evitar (talvez também por lag)</t>
+  </si>
+  <si>
+    <t>+500</t>
+  </si>
+  <si>
+    <t>+1.000.000</t>
+  </si>
+  <si>
+    <t>Os defeitos, talvez causados por lag, talvez por design prejudicaram muito a experiencia</t>
+  </si>
+  <si>
+    <t>Resposta boa dos comandos, implementação de um gesto para descer plataformas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\ \ mmm\ \ yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,8 +552,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,8 +594,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -672,8 +805,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -681,8 +829,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" applyNumberFormat="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -710,19 +859,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -748,30 +907,50 @@
     <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="16" xfId="7" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="40% - Ênfase3" xfId="4" builtinId="39"/>
     <cellStyle name="Célula de Verificação" xfId="3" builtinId="23"/>
+    <cellStyle name="Entrada" xfId="7" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Nota" xfId="5" builtinId="10"/>
     <cellStyle name="Saída" xfId="1" builtinId="21"/>
     <cellStyle name="Título 4" xfId="2" builtinId="19"/>
-    <cellStyle name="verdinhoDaTabela" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="verdinhoDaTabela" xfId="6"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -797,7 +976,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -835,9 +1014,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -870,26 +1049,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -922,26 +1084,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1114,7 +1259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1563,7 +1708,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1922,13 +2067,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:DT15"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="W15" sqref="W15"/>
+      <selection pane="topRight" activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,138 +2083,138 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:124" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34"/>
-      <c r="V3" s="34"/>
-      <c r="W3" s="34"/>
-      <c r="X3" s="34"/>
-      <c r="Y3" s="34"/>
-      <c r="Z3" s="34"/>
-      <c r="AA3" s="34"/>
-      <c r="AB3" s="34"/>
-      <c r="AC3" s="34"/>
-      <c r="AD3" s="34"/>
-      <c r="AE3" s="34"/>
-      <c r="AF3" s="34"/>
-      <c r="AG3" s="34"/>
-      <c r="AH3" s="34"/>
-      <c r="AI3" s="35"/>
-      <c r="AJ3" s="20" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="19"/>
+      <c r="W3" s="19"/>
+      <c r="X3" s="19"/>
+      <c r="Y3" s="19"/>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="19"/>
+      <c r="AI3" s="20"/>
+      <c r="AJ3" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="AK3" s="20"/>
-      <c r="AL3" s="20"/>
-      <c r="AM3" s="20"/>
-      <c r="AN3" s="20"/>
-      <c r="AO3" s="20"/>
-      <c r="AP3" s="20"/>
-      <c r="AQ3" s="20"/>
-      <c r="AR3" s="20"/>
-      <c r="AS3" s="20"/>
-      <c r="AT3" s="20"/>
-      <c r="AU3" s="20"/>
-      <c r="AV3" s="20"/>
-      <c r="AW3" s="20"/>
-      <c r="AX3" s="20"/>
-      <c r="AY3" s="20"/>
-      <c r="AZ3" s="20"/>
-      <c r="BA3" s="20"/>
-      <c r="BB3" s="20"/>
-      <c r="BC3" s="20"/>
-      <c r="BD3" s="20"/>
-      <c r="BE3" s="20"/>
-      <c r="BF3" s="20"/>
-      <c r="BG3" s="20"/>
-      <c r="BH3" s="20"/>
-      <c r="BI3" s="20"/>
-      <c r="BJ3" s="20"/>
-      <c r="BK3" s="20"/>
-      <c r="BL3" s="20"/>
-      <c r="BM3" s="20"/>
-      <c r="BN3" s="19" t="s">
+      <c r="AK3" s="23"/>
+      <c r="AL3" s="23"/>
+      <c r="AM3" s="23"/>
+      <c r="AN3" s="23"/>
+      <c r="AO3" s="23"/>
+      <c r="AP3" s="23"/>
+      <c r="AQ3" s="23"/>
+      <c r="AR3" s="23"/>
+      <c r="AS3" s="23"/>
+      <c r="AT3" s="23"/>
+      <c r="AU3" s="23"/>
+      <c r="AV3" s="23"/>
+      <c r="AW3" s="23"/>
+      <c r="AX3" s="23"/>
+      <c r="AY3" s="23"/>
+      <c r="AZ3" s="23"/>
+      <c r="BA3" s="23"/>
+      <c r="BB3" s="23"/>
+      <c r="BC3" s="23"/>
+      <c r="BD3" s="23"/>
+      <c r="BE3" s="23"/>
+      <c r="BF3" s="23"/>
+      <c r="BG3" s="23"/>
+      <c r="BH3" s="23"/>
+      <c r="BI3" s="23"/>
+      <c r="BJ3" s="23"/>
+      <c r="BK3" s="23"/>
+      <c r="BL3" s="23"/>
+      <c r="BM3" s="23"/>
+      <c r="BN3" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="BO3" s="19"/>
-      <c r="BP3" s="19"/>
-      <c r="BQ3" s="19"/>
-      <c r="BR3" s="19"/>
-      <c r="BS3" s="19"/>
-      <c r="BT3" s="19"/>
-      <c r="BU3" s="19"/>
-      <c r="BV3" s="19"/>
-      <c r="BW3" s="19"/>
-      <c r="BX3" s="19"/>
-      <c r="BY3" s="19"/>
-      <c r="BZ3" s="19"/>
-      <c r="CA3" s="19"/>
-      <c r="CB3" s="19"/>
-      <c r="CC3" s="19"/>
-      <c r="CD3" s="19"/>
-      <c r="CE3" s="19"/>
-      <c r="CF3" s="19"/>
-      <c r="CG3" s="19"/>
-      <c r="CH3" s="19"/>
-      <c r="CI3" s="19"/>
-      <c r="CJ3" s="19"/>
-      <c r="CK3" s="19"/>
-      <c r="CL3" s="19"/>
-      <c r="CM3" s="19"/>
-      <c r="CN3" s="19"/>
-      <c r="CO3" s="19"/>
-      <c r="CP3" s="19"/>
-      <c r="CQ3" s="19"/>
-      <c r="CR3" s="19"/>
-      <c r="CS3" s="19" t="s">
+      <c r="BO3" s="24"/>
+      <c r="BP3" s="24"/>
+      <c r="BQ3" s="24"/>
+      <c r="BR3" s="24"/>
+      <c r="BS3" s="24"/>
+      <c r="BT3" s="24"/>
+      <c r="BU3" s="24"/>
+      <c r="BV3" s="24"/>
+      <c r="BW3" s="24"/>
+      <c r="BX3" s="24"/>
+      <c r="BY3" s="24"/>
+      <c r="BZ3" s="24"/>
+      <c r="CA3" s="24"/>
+      <c r="CB3" s="24"/>
+      <c r="CC3" s="24"/>
+      <c r="CD3" s="24"/>
+      <c r="CE3" s="24"/>
+      <c r="CF3" s="24"/>
+      <c r="CG3" s="24"/>
+      <c r="CH3" s="24"/>
+      <c r="CI3" s="24"/>
+      <c r="CJ3" s="24"/>
+      <c r="CK3" s="24"/>
+      <c r="CL3" s="24"/>
+      <c r="CM3" s="24"/>
+      <c r="CN3" s="24"/>
+      <c r="CO3" s="24"/>
+      <c r="CP3" s="24"/>
+      <c r="CQ3" s="24"/>
+      <c r="CR3" s="24"/>
+      <c r="CS3" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="CT3" s="19"/>
-      <c r="CU3" s="19"/>
-      <c r="CV3" s="19"/>
-      <c r="CW3" s="19"/>
-      <c r="CX3" s="19"/>
-      <c r="CY3" s="19"/>
-      <c r="CZ3" s="19"/>
-      <c r="DA3" s="19"/>
-      <c r="DB3" s="19"/>
-      <c r="DC3" s="19"/>
-      <c r="DD3" s="19"/>
-      <c r="DE3" s="19"/>
-      <c r="DF3" s="19"/>
-      <c r="DG3" s="19"/>
-      <c r="DH3" s="19"/>
-      <c r="DI3" s="19"/>
-      <c r="DJ3" s="19"/>
-      <c r="DK3" s="19"/>
-      <c r="DL3" s="19"/>
-      <c r="DM3" s="19"/>
-      <c r="DN3" s="19"/>
-      <c r="DO3" s="19"/>
-      <c r="DP3" s="19"/>
-      <c r="DQ3" s="19"/>
-      <c r="DR3" s="19"/>
-      <c r="DS3" s="19"/>
-      <c r="DT3" s="19"/>
+      <c r="CT3" s="24"/>
+      <c r="CU3" s="24"/>
+      <c r="CV3" s="24"/>
+      <c r="CW3" s="24"/>
+      <c r="CX3" s="24"/>
+      <c r="CY3" s="24"/>
+      <c r="CZ3" s="24"/>
+      <c r="DA3" s="24"/>
+      <c r="DB3" s="24"/>
+      <c r="DC3" s="24"/>
+      <c r="DD3" s="24"/>
+      <c r="DE3" s="24"/>
+      <c r="DF3" s="24"/>
+      <c r="DG3" s="24"/>
+      <c r="DH3" s="24"/>
+      <c r="DI3" s="24"/>
+      <c r="DJ3" s="24"/>
+      <c r="DK3" s="24"/>
+      <c r="DL3" s="24"/>
+      <c r="DM3" s="24"/>
+      <c r="DN3" s="24"/>
+      <c r="DO3" s="24"/>
+      <c r="DP3" s="24"/>
+      <c r="DQ3" s="24"/>
+      <c r="DR3" s="24"/>
+      <c r="DS3" s="24"/>
+      <c r="DT3" s="24"/>
     </row>
     <row r="4" spans="2:124" x14ac:dyDescent="0.25">
       <c r="C4" s="6">
@@ -2517,6 +2662,7 @@
       <c r="S15" s="11"/>
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2604,39 +2750,38 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A3:AD39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="29" width="18.85546875" customWidth="1"/>
-    <col min="30" max="30" width="18.42578125" customWidth="1"/>
+    <col min="4" max="31" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:31" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="34">
         <v>43523</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="21">
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="33">
         <v>43524</v>
       </c>
-      <c r="H4" s="21"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="7">
         <v>43525</v>
       </c>
@@ -2646,20 +2791,20 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="28">
+      <c r="L4" s="30">
         <v>43530</v>
       </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="21">
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="33">
         <v>43531</v>
       </c>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21">
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33">
         <v>43532</v>
       </c>
-      <c r="S4" s="21"/>
+      <c r="S4" s="33"/>
       <c r="T4" s="7">
         <v>43533</v>
       </c>
@@ -2678,17 +2823,20 @@
       <c r="Y4" s="7">
         <v>43539</v>
       </c>
-      <c r="Z4" s="21">
+      <c r="Z4" s="33">
         <v>43542</v>
       </c>
-      <c r="AA4" s="21"/>
-      <c r="AB4" s="21">
+      <c r="AA4" s="33"/>
+      <c r="AB4" s="33">
         <v>43543</v>
       </c>
-      <c r="AC4" s="21"/>
-      <c r="AD4" s="21"/>
-    </row>
-    <row r="5" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC4" s="33"/>
+      <c r="AD4" s="33"/>
+      <c r="AE4" s="17">
+        <v>43544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2708,7 +2856,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2722,7 +2870,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2736,7 +2884,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2750,41 +2898,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="28" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="J10" s="27"/>
-    </row>
-    <row r="11" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="26"/>
+      <c r="J10" s="29"/>
+    </row>
+    <row r="11" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="J11" s="27"/>
-    </row>
-    <row r="12" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="27"/>
+      <c r="J11" s="29"/>
+    </row>
+    <row r="12" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2798,7 +2946,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2823,14 +2971,14 @@
       <c r="P13" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="R13" s="17" t="s">
+      <c r="R13" s="11" t="s">
         <v>95</v>
       </c>
       <c r="S13" s="11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2838,9 +2986,9 @@
         <v>72</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="X14" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="X14" s="11" t="s">
         <v>115</v>
       </c>
       <c r="Y14" s="11" t="s">
@@ -2849,20 +2997,23 @@
       <c r="Z14" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AA14" s="17" t="s">
+      <c r="AA14" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="AB14" s="18" t="s">
+      <c r="AB14" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AC14" s="17" t="s">
+      <c r="AC14" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="AD14" s="17" t="s">
+      <c r="AD14" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE14" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -2881,20 +3032,20 @@
       <c r="Q15" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="T15" s="17" t="s">
+      <c r="T15" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="U15" s="17" t="s">
+      <c r="U15" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="V15" s="17" t="s">
+      <c r="V15" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="W15" s="17" t="s">
+      <c r="W15" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3034,4 +3185,184 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="135.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="15">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="B6" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="15">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="H6" s="41">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="B7" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="H7" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="I7" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="J7" s="43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="B8" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="J8" s="43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="B9" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="D9" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="I9" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="J9" s="43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
implementado area descida para as profundezas inimigo acelerador investidor circulador zigzag
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="listaDeTarefasComEstimativas" sheetId="2" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="timeLineDoProjeto" sheetId="3" r:id="rId3"/>
     <sheet name="horasTrabalhadas" sheetId="4" r:id="rId4"/>
     <sheet name="mercado" sheetId="5" r:id="rId5"/>
+    <sheet name="inimigosArea1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="192">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -504,6 +505,96 @@
   </si>
   <si>
     <t>Resposta boa dos comandos, implementação de um gesto para descer plataformas</t>
+  </si>
+  <si>
+    <t>20h-22h30min</t>
+  </si>
+  <si>
+    <t>O que Acelera</t>
+  </si>
+  <si>
+    <t>Investidor</t>
+  </si>
+  <si>
+    <t>Estocador</t>
+  </si>
+  <si>
+    <t>pulador</t>
+  </si>
+  <si>
+    <t>circulador</t>
+  </si>
+  <si>
+    <t>atirador</t>
+  </si>
+  <si>
+    <t>reprodutor</t>
+  </si>
+  <si>
+    <t>fortão</t>
+  </si>
+  <si>
+    <t>defensor</t>
+  </si>
+  <si>
+    <t>voador perseguidor</t>
+  </si>
+  <si>
+    <t>voador zig zag</t>
+  </si>
+  <si>
+    <t>Caracteristica</t>
+  </si>
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Pontos de Vida</t>
+  </si>
+  <si>
+    <t>Dinheiro que cai</t>
+  </si>
+  <si>
+    <t>Inimigo Comum</t>
+  </si>
+  <si>
+    <t>Voador Comum</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>10h - 12h</t>
+  </si>
+  <si>
+    <t>10h30min-11h30min</t>
+  </si>
+  <si>
+    <t>18h - 21h</t>
+  </si>
+  <si>
+    <t>21h30min-22h30min</t>
+  </si>
+  <si>
+    <t>13h-14h30min</t>
+  </si>
+  <si>
+    <t>15h - 16h30min</t>
+  </si>
+  <si>
+    <t>15h30min - 17h</t>
+  </si>
+  <si>
+    <t>19h30min - 23h</t>
+  </si>
+  <si>
+    <t>10h-12</t>
+  </si>
+  <si>
+    <t>14h-16h</t>
+  </si>
+  <si>
+    <t>23h30min</t>
   </si>
 </sst>
 </file>
@@ -560,7 +651,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -599,8 +690,26 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -820,8 +929,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB1BBCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB1BBCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB1BBCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB1BBCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -830,8 +963,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" applyNumberFormat="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -862,55 +996,7 @@
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3"/>
@@ -941,8 +1027,77 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
+    <cellStyle name="20% - Ênfase1" xfId="8" builtinId="30"/>
     <cellStyle name="40% - Ênfase3" xfId="4" builtinId="39"/>
     <cellStyle name="Célula de Verificação" xfId="3" builtinId="23"/>
     <cellStyle name="Entrada" xfId="7" builtinId="20"/>
@@ -956,6 +1111,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC6EFCE"/>
       <color rgb="FFA1D07E"/>
       <color rgb="FF82C77C"/>
       <color rgb="FF66FF66"/>
@@ -2068,12 +2224,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:DT15"/>
+  <dimension ref="B3:DT16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="X15" sqref="X15"/>
+      <selection pane="topRight" activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,138 +2239,138 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:124" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="42"/>
+      <c r="E3" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="19"/>
-      <c r="W3" s="19"/>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
-      <c r="AA3" s="19"/>
-      <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
-      <c r="AH3" s="19"/>
-      <c r="AI3" s="20"/>
-      <c r="AJ3" s="23" t="s">
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="40"/>
+      <c r="AJ3" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="AK3" s="23"/>
-      <c r="AL3" s="23"/>
-      <c r="AM3" s="23"/>
-      <c r="AN3" s="23"/>
-      <c r="AO3" s="23"/>
-      <c r="AP3" s="23"/>
-      <c r="AQ3" s="23"/>
-      <c r="AR3" s="23"/>
-      <c r="AS3" s="23"/>
-      <c r="AT3" s="23"/>
-      <c r="AU3" s="23"/>
-      <c r="AV3" s="23"/>
-      <c r="AW3" s="23"/>
-      <c r="AX3" s="23"/>
-      <c r="AY3" s="23"/>
-      <c r="AZ3" s="23"/>
-      <c r="BA3" s="23"/>
-      <c r="BB3" s="23"/>
-      <c r="BC3" s="23"/>
-      <c r="BD3" s="23"/>
-      <c r="BE3" s="23"/>
-      <c r="BF3" s="23"/>
-      <c r="BG3" s="23"/>
-      <c r="BH3" s="23"/>
-      <c r="BI3" s="23"/>
-      <c r="BJ3" s="23"/>
-      <c r="BK3" s="23"/>
-      <c r="BL3" s="23"/>
-      <c r="BM3" s="23"/>
-      <c r="BN3" s="24" t="s">
+      <c r="AK3" s="43"/>
+      <c r="AL3" s="43"/>
+      <c r="AM3" s="43"/>
+      <c r="AN3" s="43"/>
+      <c r="AO3" s="43"/>
+      <c r="AP3" s="43"/>
+      <c r="AQ3" s="43"/>
+      <c r="AR3" s="43"/>
+      <c r="AS3" s="43"/>
+      <c r="AT3" s="43"/>
+      <c r="AU3" s="43"/>
+      <c r="AV3" s="43"/>
+      <c r="AW3" s="43"/>
+      <c r="AX3" s="43"/>
+      <c r="AY3" s="43"/>
+      <c r="AZ3" s="43"/>
+      <c r="BA3" s="43"/>
+      <c r="BB3" s="43"/>
+      <c r="BC3" s="43"/>
+      <c r="BD3" s="43"/>
+      <c r="BE3" s="43"/>
+      <c r="BF3" s="43"/>
+      <c r="BG3" s="43"/>
+      <c r="BH3" s="43"/>
+      <c r="BI3" s="43"/>
+      <c r="BJ3" s="43"/>
+      <c r="BK3" s="43"/>
+      <c r="BL3" s="43"/>
+      <c r="BM3" s="43"/>
+      <c r="BN3" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="BO3" s="24"/>
-      <c r="BP3" s="24"/>
-      <c r="BQ3" s="24"/>
-      <c r="BR3" s="24"/>
-      <c r="BS3" s="24"/>
-      <c r="BT3" s="24"/>
-      <c r="BU3" s="24"/>
-      <c r="BV3" s="24"/>
-      <c r="BW3" s="24"/>
-      <c r="BX3" s="24"/>
-      <c r="BY3" s="24"/>
-      <c r="BZ3" s="24"/>
-      <c r="CA3" s="24"/>
-      <c r="CB3" s="24"/>
-      <c r="CC3" s="24"/>
-      <c r="CD3" s="24"/>
-      <c r="CE3" s="24"/>
-      <c r="CF3" s="24"/>
-      <c r="CG3" s="24"/>
-      <c r="CH3" s="24"/>
-      <c r="CI3" s="24"/>
-      <c r="CJ3" s="24"/>
-      <c r="CK3" s="24"/>
-      <c r="CL3" s="24"/>
-      <c r="CM3" s="24"/>
-      <c r="CN3" s="24"/>
-      <c r="CO3" s="24"/>
-      <c r="CP3" s="24"/>
-      <c r="CQ3" s="24"/>
-      <c r="CR3" s="24"/>
-      <c r="CS3" s="24" t="s">
+      <c r="BO3" s="44"/>
+      <c r="BP3" s="44"/>
+      <c r="BQ3" s="44"/>
+      <c r="BR3" s="44"/>
+      <c r="BS3" s="44"/>
+      <c r="BT3" s="44"/>
+      <c r="BU3" s="44"/>
+      <c r="BV3" s="44"/>
+      <c r="BW3" s="44"/>
+      <c r="BX3" s="44"/>
+      <c r="BY3" s="44"/>
+      <c r="BZ3" s="44"/>
+      <c r="CA3" s="44"/>
+      <c r="CB3" s="44"/>
+      <c r="CC3" s="44"/>
+      <c r="CD3" s="44"/>
+      <c r="CE3" s="44"/>
+      <c r="CF3" s="44"/>
+      <c r="CG3" s="44"/>
+      <c r="CH3" s="44"/>
+      <c r="CI3" s="44"/>
+      <c r="CJ3" s="44"/>
+      <c r="CK3" s="44"/>
+      <c r="CL3" s="44"/>
+      <c r="CM3" s="44"/>
+      <c r="CN3" s="44"/>
+      <c r="CO3" s="44"/>
+      <c r="CP3" s="44"/>
+      <c r="CQ3" s="44"/>
+      <c r="CR3" s="44"/>
+      <c r="CS3" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="CT3" s="24"/>
-      <c r="CU3" s="24"/>
-      <c r="CV3" s="24"/>
-      <c r="CW3" s="24"/>
-      <c r="CX3" s="24"/>
-      <c r="CY3" s="24"/>
-      <c r="CZ3" s="24"/>
-      <c r="DA3" s="24"/>
-      <c r="DB3" s="24"/>
-      <c r="DC3" s="24"/>
-      <c r="DD3" s="24"/>
-      <c r="DE3" s="24"/>
-      <c r="DF3" s="24"/>
-      <c r="DG3" s="24"/>
-      <c r="DH3" s="24"/>
-      <c r="DI3" s="24"/>
-      <c r="DJ3" s="24"/>
-      <c r="DK3" s="24"/>
-      <c r="DL3" s="24"/>
-      <c r="DM3" s="24"/>
-      <c r="DN3" s="24"/>
-      <c r="DO3" s="24"/>
-      <c r="DP3" s="24"/>
-      <c r="DQ3" s="24"/>
-      <c r="DR3" s="24"/>
-      <c r="DS3" s="24"/>
-      <c r="DT3" s="24"/>
+      <c r="CT3" s="44"/>
+      <c r="CU3" s="44"/>
+      <c r="CV3" s="44"/>
+      <c r="CW3" s="44"/>
+      <c r="CX3" s="44"/>
+      <c r="CY3" s="44"/>
+      <c r="CZ3" s="44"/>
+      <c r="DA3" s="44"/>
+      <c r="DB3" s="44"/>
+      <c r="DC3" s="44"/>
+      <c r="DD3" s="44"/>
+      <c r="DE3" s="44"/>
+      <c r="DF3" s="44"/>
+      <c r="DG3" s="44"/>
+      <c r="DH3" s="44"/>
+      <c r="DI3" s="44"/>
+      <c r="DJ3" s="44"/>
+      <c r="DK3" s="44"/>
+      <c r="DL3" s="44"/>
+      <c r="DM3" s="44"/>
+      <c r="DN3" s="44"/>
+      <c r="DO3" s="44"/>
+      <c r="DP3" s="44"/>
+      <c r="DQ3" s="44"/>
+      <c r="DR3" s="44"/>
+      <c r="DS3" s="44"/>
+      <c r="DT3" s="44"/>
     </row>
     <row r="4" spans="2:124" x14ac:dyDescent="0.25">
       <c r="C4" s="6">
@@ -2663,6 +2819,16 @@
       <c r="V15" s="11"/>
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
+    </row>
+    <row r="16" spans="2:124" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="11"/>
+      <c r="AC16" s="11"/>
+      <c r="AD16" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2708,7 +2874,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:B12 B15">
+  <conditionalFormatting sqref="B9:B12 B15:B16">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2751,37 +2917,41 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AE39"/>
+  <dimension ref="A3:AR39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE4" sqref="AE4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="AB1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="31" width="18.85546875" customWidth="1"/>
+    <col min="4" max="31" width="19" customWidth="1"/>
+    <col min="32" max="35" width="19.140625" customWidth="1"/>
+    <col min="36" max="39" width="18.5703125" customWidth="1"/>
+    <col min="40" max="41" width="14" customWidth="1"/>
+    <col min="42" max="42" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:31" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:44" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="54">
         <v>43523</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="33">
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="45">
         <v>43524</v>
       </c>
-      <c r="H4" s="33"/>
+      <c r="H4" s="45"/>
       <c r="I4" s="7">
         <v>43525</v>
       </c>
@@ -2791,20 +2961,20 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="30">
+      <c r="L4" s="51">
         <v>43530</v>
       </c>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="33">
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="45">
         <v>43531</v>
       </c>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33">
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45">
         <v>43532</v>
       </c>
-      <c r="S4" s="33"/>
+      <c r="S4" s="45"/>
       <c r="T4" s="7">
         <v>43533</v>
       </c>
@@ -2823,20 +2993,45 @@
       <c r="Y4" s="7">
         <v>43539</v>
       </c>
-      <c r="Z4" s="33">
+      <c r="Z4" s="45">
         <v>43542</v>
       </c>
-      <c r="AA4" s="33"/>
-      <c r="AB4" s="33">
+      <c r="AA4" s="45"/>
+      <c r="AB4" s="45">
         <v>43543</v>
       </c>
-      <c r="AC4" s="33"/>
-      <c r="AD4" s="33"/>
+      <c r="AC4" s="45"/>
+      <c r="AD4" s="45"/>
       <c r="AE4" s="17">
         <v>43544</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AF4" s="18">
+        <v>43545</v>
+      </c>
+      <c r="AG4" s="45">
+        <v>43546</v>
+      </c>
+      <c r="AH4" s="45"/>
+      <c r="AI4" s="35">
+        <v>43547</v>
+      </c>
+      <c r="AJ4" s="45">
+        <v>43549</v>
+      </c>
+      <c r="AK4" s="45"/>
+      <c r="AL4" s="45"/>
+      <c r="AM4" s="45"/>
+      <c r="AN4" s="45">
+        <v>43550</v>
+      </c>
+      <c r="AO4" s="45"/>
+      <c r="AP4" s="45"/>
+      <c r="AQ4" s="51">
+        <v>43551</v>
+      </c>
+      <c r="AR4" s="53"/>
+    </row>
+    <row r="5" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2856,7 +3051,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2870,7 +3065,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2884,7 +3079,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2898,41 +3093,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="49" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="26"/>
-      <c r="J10" s="29"/>
-    </row>
-    <row r="11" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="47"/>
+      <c r="J10" s="50"/>
+    </row>
+    <row r="11" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="J11" s="29"/>
-    </row>
-    <row r="12" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="48"/>
+      <c r="J11" s="50"/>
+    </row>
+    <row r="12" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2946,7 +3141,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2978,7 +3173,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3013,7 +3208,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3045,12 +3240,54 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>101</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF16" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="AG16" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="AH16" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="AI16" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="AJ16" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="AK16" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="AL16" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM16" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="AN16" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="AO16" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="AP16" s="36" t="s">
+        <v>188</v>
+      </c>
+      <c r="AQ16" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="AR16" s="36" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3147,7 +3384,11 @@
     <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="AJ4:AM4"/>
+    <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="L4:O4"/>
@@ -3171,7 +3412,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B26">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3191,7 +3432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3209,7 +3450,7 @@
   <sheetData>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="19" t="s">
         <v>122</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -3232,134 +3473,289 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="135.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="20" t="s">
         <v>125</v>
       </c>
       <c r="D5" s="15">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="H5" s="40" t="s">
+      <c r="H5" s="24" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="20" t="s">
         <v>134</v>
       </c>
       <c r="D6" s="15">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="H6" s="41">
+      <c r="H6" s="25">
         <v>100000</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="20" t="s">
         <v>140</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="G7" s="39" t="s">
+      <c r="G7" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="J7" s="43" t="s">
+      <c r="J7" s="27" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="20" t="s">
         <v>148</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="E8" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="H8" s="40" t="s">
+      <c r="H8" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="J8" s="43" t="s">
+      <c r="J8" s="27" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="150" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="26" t="s">
         <v>154</v>
       </c>
       <c r="D9" s="15">
         <v>4.5</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="G9" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="I9" s="43" t="s">
+      <c r="I9" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="27" t="s">
         <v>160</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="7" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
+    </row>
+    <row r="6" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="34"/>
+    </row>
+    <row r="7" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="34"/>
+    </row>
+    <row r="8" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
+    </row>
+    <row r="9" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="34"/>
+    </row>
+    <row r="10" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="34"/>
+    </row>
+    <row r="11" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
+    </row>
+    <row r="12" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="34"/>
+    </row>
+    <row r="13" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
+    </row>
+    <row r="14" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="34"/>
+    </row>
+    <row r="15" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="34"/>
+    </row>
+    <row r="16" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="34"/>
+    </row>
+    <row r="17" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
fonte de mana area 9 e checkpoint area 10
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="listaDeTarefasComEstimativas" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="195">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -594,7 +594,16 @@
     <t>14h-16h</t>
   </si>
   <si>
-    <t>23h30min</t>
+    <t>15h-18h</t>
+  </si>
+  <si>
+    <t>12h30min - 16h</t>
+  </si>
+  <si>
+    <t>18h30-21h</t>
+  </si>
+  <si>
+    <t>34h30min</t>
   </si>
 </sst>
 </file>
@@ -1068,6 +1077,12 @@
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1083,13 +1098,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2226,10 +2235,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:DT16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="Z24" sqref="Z24"/>
+      <selection pane="topRight" activeCell="AG16" sqref="AG16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2829,6 +2838,9 @@
       <c r="AA16" s="11"/>
       <c r="AC16" s="11"/>
       <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
+      <c r="AF16" s="11"/>
+      <c r="AG16" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2917,26 +2929,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AR39"/>
+  <dimension ref="A3:AV39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" topLeftCell="AP1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AP28" sqref="AP28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="31" width="19" customWidth="1"/>
-    <col min="32" max="35" width="19.140625" customWidth="1"/>
-    <col min="36" max="39" width="18.5703125" customWidth="1"/>
-    <col min="40" max="41" width="14" customWidth="1"/>
-    <col min="42" max="42" width="14.7109375" customWidth="1"/>
+    <col min="4" max="48" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:44" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:48" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
@@ -2961,12 +2969,12 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="51">
+      <c r="L4" s="46">
         <v>43530</v>
       </c>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="47"/>
       <c r="P4" s="45">
         <v>43531</v>
       </c>
@@ -3026,12 +3034,20 @@
       </c>
       <c r="AO4" s="45"/>
       <c r="AP4" s="45"/>
-      <c r="AQ4" s="51">
+      <c r="AQ4" s="46">
         <v>43551</v>
       </c>
-      <c r="AR4" s="53"/>
-    </row>
-    <row r="5" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AR4" s="47"/>
+      <c r="AS4" s="7">
+        <v>43552</v>
+      </c>
+      <c r="AT4" s="45">
+        <v>43553</v>
+      </c>
+      <c r="AU4" s="45"/>
+      <c r="AV4" s="45"/>
+    </row>
+    <row r="5" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3051,7 +3067,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3065,7 +3081,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3079,7 +3095,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3093,41 +3109,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="49" t="s">
+      <c r="J9" s="51" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="J10" s="50"/>
-    </row>
-    <row r="11" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="49"/>
+      <c r="J10" s="52"/>
+    </row>
+    <row r="11" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="J11" s="50"/>
-    </row>
-    <row r="12" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="50"/>
+      <c r="J11" s="52"/>
+    </row>
+    <row r="12" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3141,7 +3157,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3173,7 +3189,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3208,7 +3224,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3240,7 +3256,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:44" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3248,7 +3264,7 @@
         <v>101</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AF16" s="11" t="s">
         <v>162</v>
@@ -3288,6 +3304,18 @@
       </c>
       <c r="AR16" s="36" t="s">
         <v>190</v>
+      </c>
+      <c r="AS16" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="AT16" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="AU16" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="AV16" s="37" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3384,7 +3412,8 @@
     <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="AT4:AV4"/>
     <mergeCell ref="AN4:AP4"/>
     <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="AJ4:AM4"/>

</xml_diff>

<commit_message>
Incluindo sons no jogo Area 1 98% concluida restando posicionar Itens e introduzir algumas funções 13 inimigos implmentados 1 boss implementado 1 Update acessivel
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="listaDeTarefasComEstimativas" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="211">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -603,7 +603,55 @@
     <t>18h30-21h</t>
   </si>
   <si>
-    <t>34h30min</t>
+    <t>9h-11h30min</t>
+  </si>
+  <si>
+    <t>15h-16h</t>
+  </si>
+  <si>
+    <t>9h-11h</t>
+  </si>
+  <si>
+    <t>10h30min - 11h45min</t>
+  </si>
+  <si>
+    <t>12h30min - 15h30min</t>
+  </si>
+  <si>
+    <t>16h-17h30min</t>
+  </si>
+  <si>
+    <t>20h-21h</t>
+  </si>
+  <si>
+    <t>23h30min-0h30min</t>
+  </si>
+  <si>
+    <t>14h-15h30min</t>
+  </si>
+  <si>
+    <t>Inserção de Audio</t>
+  </si>
+  <si>
+    <t>12h30min  -13h</t>
+  </si>
+  <si>
+    <t>13h-14h45min</t>
+  </si>
+  <si>
+    <t>55h30min</t>
+  </si>
+  <si>
+    <t>15h-17h</t>
+  </si>
+  <si>
+    <t>9h30min-11h30min</t>
+  </si>
+  <si>
+    <t>14h-15h</t>
+  </si>
+  <si>
+    <t>6h45min</t>
   </si>
 </sst>
 </file>
@@ -974,7 +1022,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -1053,6 +1101,16 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1104,6 +1162,7 @@
     <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="6" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20% - Ênfase1" xfId="8" builtinId="30"/>
@@ -1427,7 +1486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -2233,12 +2292,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:DT16"/>
+  <dimension ref="B3:DT17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="AG1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="AG16" sqref="AG16"/>
+      <selection pane="topRight" activeCell="AY17" sqref="AY17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,138 +2307,138 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:124" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="38" t="s">
+      <c r="D3" s="46"/>
+      <c r="E3" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="39"/>
-      <c r="Y3" s="39"/>
-      <c r="Z3" s="39"/>
-      <c r="AA3" s="39"/>
-      <c r="AB3" s="39"/>
-      <c r="AC3" s="39"/>
-      <c r="AD3" s="39"/>
-      <c r="AE3" s="39"/>
-      <c r="AF3" s="39"/>
-      <c r="AG3" s="39"/>
-      <c r="AH3" s="39"/>
-      <c r="AI3" s="40"/>
-      <c r="AJ3" s="43" t="s">
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="43"/>
+      <c r="S3" s="43"/>
+      <c r="T3" s="43"/>
+      <c r="U3" s="43"/>
+      <c r="V3" s="43"/>
+      <c r="W3" s="43"/>
+      <c r="X3" s="43"/>
+      <c r="Y3" s="43"/>
+      <c r="Z3" s="43"/>
+      <c r="AA3" s="43"/>
+      <c r="AB3" s="43"/>
+      <c r="AC3" s="43"/>
+      <c r="AD3" s="43"/>
+      <c r="AE3" s="43"/>
+      <c r="AF3" s="43"/>
+      <c r="AG3" s="43"/>
+      <c r="AH3" s="43"/>
+      <c r="AI3" s="44"/>
+      <c r="AJ3" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="AK3" s="43"/>
-      <c r="AL3" s="43"/>
-      <c r="AM3" s="43"/>
-      <c r="AN3" s="43"/>
-      <c r="AO3" s="43"/>
-      <c r="AP3" s="43"/>
-      <c r="AQ3" s="43"/>
-      <c r="AR3" s="43"/>
-      <c r="AS3" s="43"/>
-      <c r="AT3" s="43"/>
-      <c r="AU3" s="43"/>
-      <c r="AV3" s="43"/>
-      <c r="AW3" s="43"/>
-      <c r="AX3" s="43"/>
-      <c r="AY3" s="43"/>
-      <c r="AZ3" s="43"/>
-      <c r="BA3" s="43"/>
-      <c r="BB3" s="43"/>
-      <c r="BC3" s="43"/>
-      <c r="BD3" s="43"/>
-      <c r="BE3" s="43"/>
-      <c r="BF3" s="43"/>
-      <c r="BG3" s="43"/>
-      <c r="BH3" s="43"/>
-      <c r="BI3" s="43"/>
-      <c r="BJ3" s="43"/>
-      <c r="BK3" s="43"/>
-      <c r="BL3" s="43"/>
-      <c r="BM3" s="43"/>
-      <c r="BN3" s="44" t="s">
+      <c r="AK3" s="47"/>
+      <c r="AL3" s="47"/>
+      <c r="AM3" s="47"/>
+      <c r="AN3" s="47"/>
+      <c r="AO3" s="47"/>
+      <c r="AP3" s="47"/>
+      <c r="AQ3" s="47"/>
+      <c r="AR3" s="47"/>
+      <c r="AS3" s="47"/>
+      <c r="AT3" s="47"/>
+      <c r="AU3" s="47"/>
+      <c r="AV3" s="47"/>
+      <c r="AW3" s="47"/>
+      <c r="AX3" s="47"/>
+      <c r="AY3" s="47"/>
+      <c r="AZ3" s="47"/>
+      <c r="BA3" s="47"/>
+      <c r="BB3" s="47"/>
+      <c r="BC3" s="47"/>
+      <c r="BD3" s="47"/>
+      <c r="BE3" s="47"/>
+      <c r="BF3" s="47"/>
+      <c r="BG3" s="47"/>
+      <c r="BH3" s="47"/>
+      <c r="BI3" s="47"/>
+      <c r="BJ3" s="47"/>
+      <c r="BK3" s="47"/>
+      <c r="BL3" s="47"/>
+      <c r="BM3" s="47"/>
+      <c r="BN3" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="BO3" s="44"/>
-      <c r="BP3" s="44"/>
-      <c r="BQ3" s="44"/>
-      <c r="BR3" s="44"/>
-      <c r="BS3" s="44"/>
-      <c r="BT3" s="44"/>
-      <c r="BU3" s="44"/>
-      <c r="BV3" s="44"/>
-      <c r="BW3" s="44"/>
-      <c r="BX3" s="44"/>
-      <c r="BY3" s="44"/>
-      <c r="BZ3" s="44"/>
-      <c r="CA3" s="44"/>
-      <c r="CB3" s="44"/>
-      <c r="CC3" s="44"/>
-      <c r="CD3" s="44"/>
-      <c r="CE3" s="44"/>
-      <c r="CF3" s="44"/>
-      <c r="CG3" s="44"/>
-      <c r="CH3" s="44"/>
-      <c r="CI3" s="44"/>
-      <c r="CJ3" s="44"/>
-      <c r="CK3" s="44"/>
-      <c r="CL3" s="44"/>
-      <c r="CM3" s="44"/>
-      <c r="CN3" s="44"/>
-      <c r="CO3" s="44"/>
-      <c r="CP3" s="44"/>
-      <c r="CQ3" s="44"/>
-      <c r="CR3" s="44"/>
-      <c r="CS3" s="44" t="s">
+      <c r="BO3" s="48"/>
+      <c r="BP3" s="48"/>
+      <c r="BQ3" s="48"/>
+      <c r="BR3" s="48"/>
+      <c r="BS3" s="48"/>
+      <c r="BT3" s="48"/>
+      <c r="BU3" s="48"/>
+      <c r="BV3" s="48"/>
+      <c r="BW3" s="48"/>
+      <c r="BX3" s="48"/>
+      <c r="BY3" s="48"/>
+      <c r="BZ3" s="48"/>
+      <c r="CA3" s="48"/>
+      <c r="CB3" s="48"/>
+      <c r="CC3" s="48"/>
+      <c r="CD3" s="48"/>
+      <c r="CE3" s="48"/>
+      <c r="CF3" s="48"/>
+      <c r="CG3" s="48"/>
+      <c r="CH3" s="48"/>
+      <c r="CI3" s="48"/>
+      <c r="CJ3" s="48"/>
+      <c r="CK3" s="48"/>
+      <c r="CL3" s="48"/>
+      <c r="CM3" s="48"/>
+      <c r="CN3" s="48"/>
+      <c r="CO3" s="48"/>
+      <c r="CP3" s="48"/>
+      <c r="CQ3" s="48"/>
+      <c r="CR3" s="48"/>
+      <c r="CS3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="CT3" s="44"/>
-      <c r="CU3" s="44"/>
-      <c r="CV3" s="44"/>
-      <c r="CW3" s="44"/>
-      <c r="CX3" s="44"/>
-      <c r="CY3" s="44"/>
-      <c r="CZ3" s="44"/>
-      <c r="DA3" s="44"/>
-      <c r="DB3" s="44"/>
-      <c r="DC3" s="44"/>
-      <c r="DD3" s="44"/>
-      <c r="DE3" s="44"/>
-      <c r="DF3" s="44"/>
-      <c r="DG3" s="44"/>
-      <c r="DH3" s="44"/>
-      <c r="DI3" s="44"/>
-      <c r="DJ3" s="44"/>
-      <c r="DK3" s="44"/>
-      <c r="DL3" s="44"/>
-      <c r="DM3" s="44"/>
-      <c r="DN3" s="44"/>
-      <c r="DO3" s="44"/>
-      <c r="DP3" s="44"/>
-      <c r="DQ3" s="44"/>
-      <c r="DR3" s="44"/>
-      <c r="DS3" s="44"/>
-      <c r="DT3" s="44"/>
+      <c r="CT3" s="48"/>
+      <c r="CU3" s="48"/>
+      <c r="CV3" s="48"/>
+      <c r="CW3" s="48"/>
+      <c r="CX3" s="48"/>
+      <c r="CY3" s="48"/>
+      <c r="CZ3" s="48"/>
+      <c r="DA3" s="48"/>
+      <c r="DB3" s="48"/>
+      <c r="DC3" s="48"/>
+      <c r="DD3" s="48"/>
+      <c r="DE3" s="48"/>
+      <c r="DF3" s="48"/>
+      <c r="DG3" s="48"/>
+      <c r="DH3" s="48"/>
+      <c r="DI3" s="48"/>
+      <c r="DJ3" s="48"/>
+      <c r="DK3" s="48"/>
+      <c r="DL3" s="48"/>
+      <c r="DM3" s="48"/>
+      <c r="DN3" s="48"/>
+      <c r="DO3" s="48"/>
+      <c r="DP3" s="48"/>
+      <c r="DQ3" s="48"/>
+      <c r="DR3" s="48"/>
+      <c r="DS3" s="48"/>
+      <c r="DT3" s="48"/>
     </row>
     <row r="4" spans="2:124" x14ac:dyDescent="0.25">
       <c r="C4" s="6">
@@ -2841,6 +2900,24 @@
       <c r="AE16" s="11"/>
       <c r="AF16" s="11"/>
       <c r="AG16" s="11"/>
+      <c r="AJ16" s="11"/>
+      <c r="AK16" s="11"/>
+      <c r="AL16" s="11"/>
+      <c r="AM16" s="11"/>
+      <c r="AN16" s="11"/>
+      <c r="AQ16" s="11"/>
+      <c r="AR16" s="11"/>
+      <c r="AS16" s="11"/>
+      <c r="AT16" s="11"/>
+      <c r="AU16" s="11"/>
+    </row>
+    <row r="17" spans="2:51" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>203</v>
+      </c>
+      <c r="AV17" s="11"/>
+      <c r="AX17" s="11"/>
+      <c r="AY17" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2851,6 +2928,18 @@
     <mergeCell ref="CS3:DT3"/>
   </mergeCells>
   <conditionalFormatting sqref="B6">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -2862,7 +2951,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
+  <conditionalFormatting sqref="B8">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -2874,8 +2963,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="B9:B12 B15:B16">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2886,7 +2975,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:B12 B15:B16">
+  <conditionalFormatting sqref="B13">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2898,7 +2987,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
+  <conditionalFormatting sqref="B14">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2910,7 +2999,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14">
+  <conditionalFormatting sqref="B17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2929,11 +3018,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AV39"/>
+  <dimension ref="A3:BQ39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP28" sqref="AP28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="BF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2941,25 +3030,39 @@
     <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="48" width="17.85546875" customWidth="1"/>
+    <col min="49" max="50" width="12.5703125" customWidth="1"/>
+    <col min="51" max="51" width="10.5703125" customWidth="1"/>
+    <col min="52" max="52" width="19.85546875" customWidth="1"/>
+    <col min="54" max="54" width="18.85546875" customWidth="1"/>
+    <col min="55" max="55" width="19.5703125" customWidth="1"/>
+    <col min="56" max="59" width="18.42578125" customWidth="1"/>
+    <col min="60" max="60" width="18.5703125" customWidth="1"/>
+    <col min="61" max="61" width="17.5703125" customWidth="1"/>
+    <col min="62" max="63" width="17.85546875" customWidth="1"/>
+    <col min="64" max="64" width="18.5703125" customWidth="1"/>
+    <col min="65" max="65" width="14.85546875" customWidth="1"/>
+    <col min="66" max="66" width="13.7109375" customWidth="1"/>
+    <col min="68" max="68" width="18.140625" customWidth="1"/>
+    <col min="69" max="69" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:48" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:69" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="58">
         <v>43523</v>
       </c>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="45">
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="49">
         <v>43524</v>
       </c>
-      <c r="H4" s="45"/>
+      <c r="H4" s="49"/>
       <c r="I4" s="7">
         <v>43525</v>
       </c>
@@ -2969,20 +3072,20 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="46">
+      <c r="L4" s="50">
         <v>43530</v>
       </c>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="45">
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="49">
         <v>43531</v>
       </c>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45">
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49">
         <v>43532</v>
       </c>
-      <c r="S4" s="45"/>
+      <c r="S4" s="49"/>
       <c r="T4" s="7">
         <v>43533</v>
       </c>
@@ -3001,53 +3104,100 @@
       <c r="Y4" s="7">
         <v>43539</v>
       </c>
-      <c r="Z4" s="45">
+      <c r="Z4" s="49">
         <v>43542</v>
       </c>
-      <c r="AA4" s="45"/>
-      <c r="AB4" s="45">
+      <c r="AA4" s="49"/>
+      <c r="AB4" s="49">
         <v>43543</v>
       </c>
-      <c r="AC4" s="45"/>
-      <c r="AD4" s="45"/>
+      <c r="AC4" s="49"/>
+      <c r="AD4" s="49"/>
       <c r="AE4" s="17">
         <v>43544</v>
       </c>
       <c r="AF4" s="18">
         <v>43545</v>
       </c>
-      <c r="AG4" s="45">
+      <c r="AG4" s="49">
         <v>43546</v>
       </c>
-      <c r="AH4" s="45"/>
+      <c r="AH4" s="49"/>
       <c r="AI4" s="35">
         <v>43547</v>
       </c>
-      <c r="AJ4" s="45">
+      <c r="AJ4" s="49">
         <v>43549</v>
       </c>
-      <c r="AK4" s="45"/>
-      <c r="AL4" s="45"/>
-      <c r="AM4" s="45"/>
-      <c r="AN4" s="45">
+      <c r="AK4" s="49"/>
+      <c r="AL4" s="49"/>
+      <c r="AM4" s="49"/>
+      <c r="AN4" s="49">
         <v>43550</v>
       </c>
-      <c r="AO4" s="45"/>
-      <c r="AP4" s="45"/>
-      <c r="AQ4" s="46">
+      <c r="AO4" s="49"/>
+      <c r="AP4" s="49"/>
+      <c r="AQ4" s="50">
         <v>43551</v>
       </c>
-      <c r="AR4" s="47"/>
+      <c r="AR4" s="51"/>
       <c r="AS4" s="7">
         <v>43552</v>
       </c>
-      <c r="AT4" s="45">
+      <c r="AT4" s="49">
         <v>43553</v>
       </c>
-      <c r="AU4" s="45"/>
-      <c r="AV4" s="45"/>
-    </row>
-    <row r="5" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AU4" s="49"/>
+      <c r="AV4" s="49"/>
+      <c r="AW4" s="50">
+        <v>43556</v>
+      </c>
+      <c r="AX4" s="51"/>
+      <c r="AY4" s="38">
+        <v>43557</v>
+      </c>
+      <c r="AZ4" s="38">
+        <v>43558</v>
+      </c>
+      <c r="BA4" s="7">
+        <v>43559</v>
+      </c>
+      <c r="BB4" s="49">
+        <v>43560</v>
+      </c>
+      <c r="BC4" s="49"/>
+      <c r="BD4" s="39">
+        <v>43563</v>
+      </c>
+      <c r="BE4" s="49">
+        <v>43564</v>
+      </c>
+      <c r="BF4" s="49"/>
+      <c r="BG4" s="49"/>
+      <c r="BH4" s="49">
+        <v>43565</v>
+      </c>
+      <c r="BI4" s="49"/>
+      <c r="BJ4" s="49">
+        <v>43566</v>
+      </c>
+      <c r="BK4" s="49"/>
+      <c r="BL4" s="49">
+        <v>43567</v>
+      </c>
+      <c r="BM4" s="49"/>
+      <c r="BN4" s="7">
+        <v>43568</v>
+      </c>
+      <c r="BO4" s="7">
+        <v>43570</v>
+      </c>
+      <c r="BP4" s="49">
+        <v>43571</v>
+      </c>
+      <c r="BQ4" s="49"/>
+    </row>
+    <row r="5" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3066,8 +3216,10 @@
       <c r="F5" s="10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="6" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BD5" s="40"/>
+      <c r="BE5" s="40"/>
+    </row>
+    <row r="6" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3081,7 +3233,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3095,7 +3247,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3109,41 +3261,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="51" t="s">
+      <c r="J9" s="55" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="J10" s="52"/>
-    </row>
-    <row r="11" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="53"/>
+      <c r="J10" s="56"/>
+    </row>
+    <row r="11" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="J11" s="52"/>
-    </row>
-    <row r="12" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="54"/>
+      <c r="J11" s="56"/>
+    </row>
+    <row r="12" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3157,7 +3309,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3189,7 +3341,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3224,7 +3376,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3256,7 +3408,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:48" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3264,7 +3416,7 @@
         <v>101</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="AF16" s="11" t="s">
         <v>162</v>
@@ -3317,93 +3469,163 @@
       <c r="AV16" s="37" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AW16" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="AX16" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="AY16" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="AZ16" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="BA16" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="BB16" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="BC16" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="BD16" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="BE16" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="BF16" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="BG16" s="37" t="s">
+        <v>200</v>
+      </c>
+      <c r="BH16" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="BI16" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="BJ16" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="BK16" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="BL16" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="BM16" s="37" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>210</v>
+      </c>
+      <c r="BN17" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="BO17" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="BP17" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="BQ17" s="59" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
-      <c r="B19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
-      <c r="B24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3412,12 +3634,10 @@
     <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="AJ4:AM4"/>
-    <mergeCell ref="AG4:AH4"/>
+  <mergeCells count="21">
+    <mergeCell ref="BL4:BM4"/>
+    <mergeCell ref="BJ4:BK4"/>
+    <mergeCell ref="BP4:BQ4"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="L4:O4"/>
@@ -3427,6 +3647,15 @@
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="G4:H4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="BH4:BI4"/>
+    <mergeCell ref="BE4:BG4"/>
+    <mergeCell ref="BB4:BC4"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="AJ4:AM4"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A26">
     <cfRule type="colorScale" priority="8">
@@ -3440,8 +3669,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:B26">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="B5:B27">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Inserindo funções dos dois emblemas iniciais
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="211">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -651,7 +651,7 @@
     <t>14h-15h</t>
   </si>
   <si>
-    <t>6h45min</t>
+    <t>7h45min</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1135,12 +1135,6 @@
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1156,13 +1150,19 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20% - Ênfase1" xfId="8" builtinId="30"/>
@@ -3018,7 +3018,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:BQ39"/>
+  <dimension ref="A3:BR39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="BF1" activePane="topRight" state="frozen"/>
@@ -3046,8 +3046,8 @@
     <col min="69" max="69" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:69" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:70" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
@@ -3072,12 +3072,12 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="50">
+      <c r="L4" s="55">
         <v>43530</v>
       </c>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="51"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="57"/>
       <c r="P4" s="49">
         <v>43531</v>
       </c>
@@ -3137,10 +3137,10 @@
       </c>
       <c r="AO4" s="49"/>
       <c r="AP4" s="49"/>
-      <c r="AQ4" s="50">
+      <c r="AQ4" s="55">
         <v>43551</v>
       </c>
-      <c r="AR4" s="51"/>
+      <c r="AR4" s="57"/>
       <c r="AS4" s="7">
         <v>43552</v>
       </c>
@@ -3149,10 +3149,10 @@
       </c>
       <c r="AU4" s="49"/>
       <c r="AV4" s="49"/>
-      <c r="AW4" s="50">
+      <c r="AW4" s="55">
         <v>43556</v>
       </c>
-      <c r="AX4" s="51"/>
+      <c r="AX4" s="57"/>
       <c r="AY4" s="38">
         <v>43557</v>
       </c>
@@ -3196,8 +3196,11 @@
         <v>43571</v>
       </c>
       <c r="BQ4" s="49"/>
-    </row>
-    <row r="5" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BR4" s="59">
+        <v>43572</v>
+      </c>
+    </row>
+    <row r="5" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3219,7 +3222,7 @@
       <c r="BD5" s="40"/>
       <c r="BE5" s="40"/>
     </row>
-    <row r="6" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3233,7 +3236,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3247,7 +3250,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3261,41 +3264,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="55" t="s">
+      <c r="J9" s="53" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="J10" s="56"/>
-    </row>
-    <row r="11" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="51"/>
+      <c r="J10" s="54"/>
+    </row>
+    <row r="11" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="J11" s="56"/>
-    </row>
-    <row r="12" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="52"/>
+      <c r="J11" s="54"/>
+    </row>
+    <row r="12" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3341,7 +3344,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3376,7 +3379,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3408,7 +3411,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3521,14 +3524,14 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="B17" t="s">
         <v>203</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="15" t="s">
         <v>210</v>
       </c>
       <c r="BN17" s="11" t="s">
@@ -3540,11 +3543,14 @@
       <c r="BP17" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="BQ17" s="59" t="s">
+      <c r="BQ17" s="41" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="18" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BR17" s="41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -3552,7 +3558,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -3560,7 +3566,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3568,7 +3574,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -3576,7 +3582,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3584,7 +3590,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -3592,7 +3598,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -3600,7 +3606,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -3608,7 +3614,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -3616,16 +3622,16 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:69" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3635,6 +3641,11 @@
     <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="AJ4:AM4"/>
     <mergeCell ref="BL4:BM4"/>
     <mergeCell ref="BJ4:BK4"/>
     <mergeCell ref="BP4:BQ4"/>
@@ -3651,11 +3662,6 @@
     <mergeCell ref="BH4:BI4"/>
     <mergeCell ref="BE4:BG4"/>
     <mergeCell ref="BB4:BC4"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="AJ4:AM4"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A26">
     <cfRule type="colorScale" priority="8">

</xml_diff>

<commit_message>
no caminho de terminar o shop de herika
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="listaDeTarefasComEstimativas" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="213">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -639,9 +639,6 @@
     <t>13h-14h45min</t>
   </si>
   <si>
-    <t>55h30min</t>
-  </si>
-  <si>
     <t>15h-17h</t>
   </si>
   <si>
@@ -651,7 +648,16 @@
     <t>14h-15h</t>
   </si>
   <si>
-    <t>7h45min</t>
+    <t>19h30-21h</t>
+  </si>
+  <si>
+    <t>8h45min</t>
+  </si>
+  <si>
+    <t>10h11h</t>
+  </si>
+  <si>
+    <t>61h</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1028,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -1111,6 +1117,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1132,6 +1147,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1150,19 +1171,13 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="20% - Ênfase1" xfId="8" builtinId="30"/>
@@ -2294,10 +2309,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:DT17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AG1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="AY17" sqref="AY17"/>
+      <selection pane="topRight" activeCell="BM9" sqref="BM9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2307,138 +2322,138 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:124" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="42" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
-      <c r="W3" s="43"/>
-      <c r="X3" s="43"/>
-      <c r="Y3" s="43"/>
-      <c r="Z3" s="43"/>
-      <c r="AA3" s="43"/>
-      <c r="AB3" s="43"/>
-      <c r="AC3" s="43"/>
-      <c r="AD3" s="43"/>
-      <c r="AE3" s="43"/>
-      <c r="AF3" s="43"/>
-      <c r="AG3" s="43"/>
-      <c r="AH3" s="43"/>
-      <c r="AI3" s="44"/>
-      <c r="AJ3" s="47" t="s">
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="46"/>
+      <c r="AB3" s="46"/>
+      <c r="AC3" s="46"/>
+      <c r="AD3" s="46"/>
+      <c r="AE3" s="46"/>
+      <c r="AF3" s="46"/>
+      <c r="AG3" s="46"/>
+      <c r="AH3" s="46"/>
+      <c r="AI3" s="47"/>
+      <c r="AJ3" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="AK3" s="47"/>
-      <c r="AL3" s="47"/>
-      <c r="AM3" s="47"/>
-      <c r="AN3" s="47"/>
-      <c r="AO3" s="47"/>
-      <c r="AP3" s="47"/>
-      <c r="AQ3" s="47"/>
-      <c r="AR3" s="47"/>
-      <c r="AS3" s="47"/>
-      <c r="AT3" s="47"/>
-      <c r="AU3" s="47"/>
-      <c r="AV3" s="47"/>
-      <c r="AW3" s="47"/>
-      <c r="AX3" s="47"/>
-      <c r="AY3" s="47"/>
-      <c r="AZ3" s="47"/>
-      <c r="BA3" s="47"/>
-      <c r="BB3" s="47"/>
-      <c r="BC3" s="47"/>
-      <c r="BD3" s="47"/>
-      <c r="BE3" s="47"/>
-      <c r="BF3" s="47"/>
-      <c r="BG3" s="47"/>
-      <c r="BH3" s="47"/>
-      <c r="BI3" s="47"/>
-      <c r="BJ3" s="47"/>
-      <c r="BK3" s="47"/>
-      <c r="BL3" s="47"/>
-      <c r="BM3" s="47"/>
-      <c r="BN3" s="48" t="s">
+      <c r="AK3" s="50"/>
+      <c r="AL3" s="50"/>
+      <c r="AM3" s="50"/>
+      <c r="AN3" s="50"/>
+      <c r="AO3" s="50"/>
+      <c r="AP3" s="50"/>
+      <c r="AQ3" s="50"/>
+      <c r="AR3" s="50"/>
+      <c r="AS3" s="50"/>
+      <c r="AT3" s="50"/>
+      <c r="AU3" s="50"/>
+      <c r="AV3" s="50"/>
+      <c r="AW3" s="50"/>
+      <c r="AX3" s="50"/>
+      <c r="AY3" s="50"/>
+      <c r="AZ3" s="50"/>
+      <c r="BA3" s="50"/>
+      <c r="BB3" s="50"/>
+      <c r="BC3" s="50"/>
+      <c r="BD3" s="50"/>
+      <c r="BE3" s="50"/>
+      <c r="BF3" s="50"/>
+      <c r="BG3" s="50"/>
+      <c r="BH3" s="50"/>
+      <c r="BI3" s="50"/>
+      <c r="BJ3" s="50"/>
+      <c r="BK3" s="50"/>
+      <c r="BL3" s="50"/>
+      <c r="BM3" s="50"/>
+      <c r="BN3" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="BO3" s="48"/>
-      <c r="BP3" s="48"/>
-      <c r="BQ3" s="48"/>
-      <c r="BR3" s="48"/>
-      <c r="BS3" s="48"/>
-      <c r="BT3" s="48"/>
-      <c r="BU3" s="48"/>
-      <c r="BV3" s="48"/>
-      <c r="BW3" s="48"/>
-      <c r="BX3" s="48"/>
-      <c r="BY3" s="48"/>
-      <c r="BZ3" s="48"/>
-      <c r="CA3" s="48"/>
-      <c r="CB3" s="48"/>
-      <c r="CC3" s="48"/>
-      <c r="CD3" s="48"/>
-      <c r="CE3" s="48"/>
-      <c r="CF3" s="48"/>
-      <c r="CG3" s="48"/>
-      <c r="CH3" s="48"/>
-      <c r="CI3" s="48"/>
-      <c r="CJ3" s="48"/>
-      <c r="CK3" s="48"/>
-      <c r="CL3" s="48"/>
-      <c r="CM3" s="48"/>
-      <c r="CN3" s="48"/>
-      <c r="CO3" s="48"/>
-      <c r="CP3" s="48"/>
-      <c r="CQ3" s="48"/>
-      <c r="CR3" s="48"/>
-      <c r="CS3" s="48" t="s">
+      <c r="BO3" s="51"/>
+      <c r="BP3" s="51"/>
+      <c r="BQ3" s="51"/>
+      <c r="BR3" s="51"/>
+      <c r="BS3" s="51"/>
+      <c r="BT3" s="51"/>
+      <c r="BU3" s="51"/>
+      <c r="BV3" s="51"/>
+      <c r="BW3" s="51"/>
+      <c r="BX3" s="51"/>
+      <c r="BY3" s="51"/>
+      <c r="BZ3" s="51"/>
+      <c r="CA3" s="51"/>
+      <c r="CB3" s="51"/>
+      <c r="CC3" s="51"/>
+      <c r="CD3" s="51"/>
+      <c r="CE3" s="51"/>
+      <c r="CF3" s="51"/>
+      <c r="CG3" s="51"/>
+      <c r="CH3" s="51"/>
+      <c r="CI3" s="51"/>
+      <c r="CJ3" s="51"/>
+      <c r="CK3" s="51"/>
+      <c r="CL3" s="51"/>
+      <c r="CM3" s="51"/>
+      <c r="CN3" s="51"/>
+      <c r="CO3" s="51"/>
+      <c r="CP3" s="51"/>
+      <c r="CQ3" s="51"/>
+      <c r="CR3" s="51"/>
+      <c r="CS3" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="CT3" s="48"/>
-      <c r="CU3" s="48"/>
-      <c r="CV3" s="48"/>
-      <c r="CW3" s="48"/>
-      <c r="CX3" s="48"/>
-      <c r="CY3" s="48"/>
-      <c r="CZ3" s="48"/>
-      <c r="DA3" s="48"/>
-      <c r="DB3" s="48"/>
-      <c r="DC3" s="48"/>
-      <c r="DD3" s="48"/>
-      <c r="DE3" s="48"/>
-      <c r="DF3" s="48"/>
-      <c r="DG3" s="48"/>
-      <c r="DH3" s="48"/>
-      <c r="DI3" s="48"/>
-      <c r="DJ3" s="48"/>
-      <c r="DK3" s="48"/>
-      <c r="DL3" s="48"/>
-      <c r="DM3" s="48"/>
-      <c r="DN3" s="48"/>
-      <c r="DO3" s="48"/>
-      <c r="DP3" s="48"/>
-      <c r="DQ3" s="48"/>
-      <c r="DR3" s="48"/>
-      <c r="DS3" s="48"/>
-      <c r="DT3" s="48"/>
+      <c r="CT3" s="51"/>
+      <c r="CU3" s="51"/>
+      <c r="CV3" s="51"/>
+      <c r="CW3" s="51"/>
+      <c r="CX3" s="51"/>
+      <c r="CY3" s="51"/>
+      <c r="CZ3" s="51"/>
+      <c r="DA3" s="51"/>
+      <c r="DB3" s="51"/>
+      <c r="DC3" s="51"/>
+      <c r="DD3" s="51"/>
+      <c r="DE3" s="51"/>
+      <c r="DF3" s="51"/>
+      <c r="DG3" s="51"/>
+      <c r="DH3" s="51"/>
+      <c r="DI3" s="51"/>
+      <c r="DJ3" s="51"/>
+      <c r="DK3" s="51"/>
+      <c r="DL3" s="51"/>
+      <c r="DM3" s="51"/>
+      <c r="DN3" s="51"/>
+      <c r="DO3" s="51"/>
+      <c r="DP3" s="51"/>
+      <c r="DQ3" s="51"/>
+      <c r="DR3" s="51"/>
+      <c r="DS3" s="51"/>
+      <c r="DT3" s="51"/>
     </row>
     <row r="4" spans="2:124" x14ac:dyDescent="0.25">
       <c r="C4" s="6">
@@ -2910,14 +2925,21 @@
       <c r="AS16" s="11"/>
       <c r="AT16" s="11"/>
       <c r="AU16" s="11"/>
-    </row>
-    <row r="17" spans="2:51" x14ac:dyDescent="0.25">
+      <c r="BA16" s="11"/>
+      <c r="BE16" s="11"/>
+      <c r="BF16" s="11"/>
+      <c r="BI16" s="11"/>
+      <c r="BL16" s="11"/>
+      <c r="BM16" s="11"/>
+    </row>
+    <row r="17" spans="2:52" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>203</v>
       </c>
       <c r="AV17" s="11"/>
       <c r="AX17" s="11"/>
       <c r="AY17" s="11"/>
+      <c r="AZ17" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3018,11 +3040,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:BR39"/>
+  <dimension ref="A3:BX39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="BF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BW4" sqref="BW4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3044,25 +3066,27 @@
     <col min="66" max="66" width="13.7109375" customWidth="1"/>
     <col min="68" max="68" width="18.140625" customWidth="1"/>
     <col min="69" max="69" width="11.7109375" customWidth="1"/>
+    <col min="73" max="73" width="11.28515625" customWidth="1"/>
+    <col min="75" max="75" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:70" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:70" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:76" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:76" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="58">
+      <c r="D4" s="61">
         <v>43523</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="49">
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="54">
         <v>43524</v>
       </c>
-      <c r="H4" s="49"/>
+      <c r="H4" s="54"/>
       <c r="I4" s="7">
         <v>43525</v>
       </c>
@@ -3072,20 +3096,20 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="55">
+      <c r="L4" s="52">
         <v>43530</v>
       </c>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="49">
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="54">
         <v>43531</v>
       </c>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="49">
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54">
         <v>43532</v>
       </c>
-      <c r="S4" s="49"/>
+      <c r="S4" s="54"/>
       <c r="T4" s="7">
         <v>43533</v>
       </c>
@@ -3104,55 +3128,55 @@
       <c r="Y4" s="7">
         <v>43539</v>
       </c>
-      <c r="Z4" s="49">
+      <c r="Z4" s="54">
         <v>43542</v>
       </c>
-      <c r="AA4" s="49"/>
-      <c r="AB4" s="49">
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="54">
         <v>43543</v>
       </c>
-      <c r="AC4" s="49"/>
-      <c r="AD4" s="49"/>
+      <c r="AC4" s="54"/>
+      <c r="AD4" s="54"/>
       <c r="AE4" s="17">
         <v>43544</v>
       </c>
       <c r="AF4" s="18">
         <v>43545</v>
       </c>
-      <c r="AG4" s="49">
+      <c r="AG4" s="54">
         <v>43546</v>
       </c>
-      <c r="AH4" s="49"/>
+      <c r="AH4" s="54"/>
       <c r="AI4" s="35">
         <v>43547</v>
       </c>
-      <c r="AJ4" s="49">
+      <c r="AJ4" s="54">
         <v>43549</v>
       </c>
-      <c r="AK4" s="49"/>
-      <c r="AL4" s="49"/>
-      <c r="AM4" s="49"/>
-      <c r="AN4" s="49">
+      <c r="AK4" s="54"/>
+      <c r="AL4" s="54"/>
+      <c r="AM4" s="54"/>
+      <c r="AN4" s="54">
         <v>43550</v>
       </c>
-      <c r="AO4" s="49"/>
-      <c r="AP4" s="49"/>
-      <c r="AQ4" s="55">
+      <c r="AO4" s="54"/>
+      <c r="AP4" s="54"/>
+      <c r="AQ4" s="52">
         <v>43551</v>
       </c>
-      <c r="AR4" s="57"/>
+      <c r="AR4" s="53"/>
       <c r="AS4" s="7">
         <v>43552</v>
       </c>
-      <c r="AT4" s="49">
+      <c r="AT4" s="54">
         <v>43553</v>
       </c>
-      <c r="AU4" s="49"/>
-      <c r="AV4" s="49"/>
-      <c r="AW4" s="55">
+      <c r="AU4" s="54"/>
+      <c r="AV4" s="54"/>
+      <c r="AW4" s="52">
         <v>43556</v>
       </c>
-      <c r="AX4" s="57"/>
+      <c r="AX4" s="53"/>
       <c r="AY4" s="38">
         <v>43557</v>
       </c>
@@ -3162,45 +3186,63 @@
       <c r="BA4" s="7">
         <v>43559</v>
       </c>
-      <c r="BB4" s="49">
+      <c r="BB4" s="54">
         <v>43560</v>
       </c>
-      <c r="BC4" s="49"/>
+      <c r="BC4" s="54"/>
       <c r="BD4" s="39">
         <v>43563</v>
       </c>
-      <c r="BE4" s="49">
+      <c r="BE4" s="54">
         <v>43564</v>
       </c>
-      <c r="BF4" s="49"/>
-      <c r="BG4" s="49"/>
-      <c r="BH4" s="49">
+      <c r="BF4" s="54"/>
+      <c r="BG4" s="54"/>
+      <c r="BH4" s="54">
         <v>43565</v>
       </c>
-      <c r="BI4" s="49"/>
-      <c r="BJ4" s="49">
+      <c r="BI4" s="54"/>
+      <c r="BJ4" s="54">
         <v>43566</v>
       </c>
-      <c r="BK4" s="49"/>
-      <c r="BL4" s="49">
+      <c r="BK4" s="54"/>
+      <c r="BL4" s="54">
         <v>43567</v>
       </c>
-      <c r="BM4" s="49"/>
+      <c r="BM4" s="54"/>
       <c r="BN4" s="7">
         <v>43568</v>
       </c>
       <c r="BO4" s="7">
         <v>43570</v>
       </c>
-      <c r="BP4" s="49">
+      <c r="BP4" s="54">
         <v>43571</v>
       </c>
-      <c r="BQ4" s="49"/>
-      <c r="BR4" s="59">
+      <c r="BQ4" s="54"/>
+      <c r="BR4" s="42">
         <v>43572</v>
       </c>
-    </row>
-    <row r="5" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BS4" s="42">
+        <v>43573</v>
+      </c>
+      <c r="BT4" s="7">
+        <v>43577</v>
+      </c>
+      <c r="BU4" s="7">
+        <v>43578</v>
+      </c>
+      <c r="BV4" s="7">
+        <v>43581</v>
+      </c>
+      <c r="BW4" s="44">
+        <v>43584</v>
+      </c>
+      <c r="BX4" s="7">
+        <v>43585</v>
+      </c>
+    </row>
+    <row r="5" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3222,7 +3264,7 @@
       <c r="BD5" s="40"/>
       <c r="BE5" s="40"/>
     </row>
-    <row r="6" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3236,7 +3278,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3250,7 +3292,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3264,41 +3306,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="53" t="s">
+      <c r="J9" s="58" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="J10" s="54"/>
-    </row>
-    <row r="11" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="56"/>
+      <c r="J10" s="59"/>
+    </row>
+    <row r="11" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="52"/>
-      <c r="J11" s="54"/>
-    </row>
-    <row r="12" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="57"/>
+      <c r="J11" s="59"/>
+    </row>
+    <row r="12" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3312,7 +3354,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3344,7 +3386,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3379,7 +3421,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3411,15 +3453,15 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:76" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>206</v>
+      <c r="C16" s="43" t="s">
+        <v>212</v>
       </c>
       <c r="AF16" s="11" t="s">
         <v>162</v>
@@ -3523,8 +3565,23 @@
       <c r="BM16" s="37" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="17" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BT16" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="BU16" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="BV16" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="BW16" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="BX16" s="62" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -3538,19 +3595,22 @@
         <v>205</v>
       </c>
       <c r="BO17" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="BP17" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="BP17" s="11" t="s">
+      <c r="BQ17" s="41" t="s">
         <v>208</v>
-      </c>
-      <c r="BQ17" s="41" t="s">
-        <v>209</v>
       </c>
       <c r="BR17" s="41" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="18" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BS17" s="41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -3558,7 +3618,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -3566,7 +3626,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3574,7 +3634,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -3582,7 +3642,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3590,7 +3650,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -3598,7 +3658,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -3606,7 +3666,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -3614,7 +3674,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -3622,16 +3682,19 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>23</v>
+      </c>
       <c r="B27" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:70" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:71" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3641,11 +3704,6 @@
     <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="AJ4:AM4"/>
     <mergeCell ref="BL4:BM4"/>
     <mergeCell ref="BJ4:BK4"/>
     <mergeCell ref="BP4:BQ4"/>
@@ -3662,8 +3720,13 @@
     <mergeCell ref="BH4:BI4"/>
     <mergeCell ref="BE4:BG4"/>
     <mergeCell ref="BB4:BC4"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="AJ4:AM4"/>
   </mergeCells>
-  <conditionalFormatting sqref="A5:A26">
+  <conditionalFormatting sqref="A5:A27">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
aquifero do buscador preparacao para a subida
implementacao do voador investidor
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="222">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -669,7 +669,22 @@
     <t>20h-23h</t>
   </si>
   <si>
-    <t>3h</t>
+    <t>10h-12h</t>
+  </si>
+  <si>
+    <t>18h-20h</t>
+  </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>19h-21h</t>
+  </si>
+  <si>
+    <t>21h30min-23h</t>
+  </si>
+  <si>
+    <t>8h30min</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1055,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
@@ -1139,6 +1154,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2322,9 +2340,9 @@
   <dimension ref="B3:DT18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AO1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="AV1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="BO17" sqref="BO17"/>
+      <selection pane="topRight" activeCell="BZ17" sqref="BZ17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2334,138 +2352,138 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:124" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="46" t="s">
+      <c r="D3" s="51"/>
+      <c r="E3" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-      <c r="S3" s="47"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="47"/>
-      <c r="Y3" s="47"/>
-      <c r="Z3" s="47"/>
-      <c r="AA3" s="47"/>
-      <c r="AB3" s="47"/>
-      <c r="AC3" s="47"/>
-      <c r="AD3" s="47"/>
-      <c r="AE3" s="47"/>
-      <c r="AF3" s="47"/>
-      <c r="AG3" s="47"/>
-      <c r="AH3" s="47"/>
-      <c r="AI3" s="48"/>
-      <c r="AJ3" s="51" t="s">
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+      <c r="AC3" s="48"/>
+      <c r="AD3" s="48"/>
+      <c r="AE3" s="48"/>
+      <c r="AF3" s="48"/>
+      <c r="AG3" s="48"/>
+      <c r="AH3" s="48"/>
+      <c r="AI3" s="49"/>
+      <c r="AJ3" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="51"/>
-      <c r="AM3" s="51"/>
-      <c r="AN3" s="51"/>
-      <c r="AO3" s="51"/>
-      <c r="AP3" s="51"/>
-      <c r="AQ3" s="51"/>
-      <c r="AR3" s="51"/>
-      <c r="AS3" s="51"/>
-      <c r="AT3" s="51"/>
-      <c r="AU3" s="51"/>
-      <c r="AV3" s="51"/>
-      <c r="AW3" s="51"/>
-      <c r="AX3" s="51"/>
-      <c r="AY3" s="51"/>
-      <c r="AZ3" s="51"/>
-      <c r="BA3" s="51"/>
-      <c r="BB3" s="51"/>
-      <c r="BC3" s="51"/>
-      <c r="BD3" s="51"/>
-      <c r="BE3" s="51"/>
-      <c r="BF3" s="51"/>
-      <c r="BG3" s="51"/>
-      <c r="BH3" s="51"/>
-      <c r="BI3" s="51"/>
-      <c r="BJ3" s="51"/>
-      <c r="BK3" s="51"/>
-      <c r="BL3" s="51"/>
-      <c r="BM3" s="51"/>
-      <c r="BN3" s="52" t="s">
+      <c r="AK3" s="52"/>
+      <c r="AL3" s="52"/>
+      <c r="AM3" s="52"/>
+      <c r="AN3" s="52"/>
+      <c r="AO3" s="52"/>
+      <c r="AP3" s="52"/>
+      <c r="AQ3" s="52"/>
+      <c r="AR3" s="52"/>
+      <c r="AS3" s="52"/>
+      <c r="AT3" s="52"/>
+      <c r="AU3" s="52"/>
+      <c r="AV3" s="52"/>
+      <c r="AW3" s="52"/>
+      <c r="AX3" s="52"/>
+      <c r="AY3" s="52"/>
+      <c r="AZ3" s="52"/>
+      <c r="BA3" s="52"/>
+      <c r="BB3" s="52"/>
+      <c r="BC3" s="52"/>
+      <c r="BD3" s="52"/>
+      <c r="BE3" s="52"/>
+      <c r="BF3" s="52"/>
+      <c r="BG3" s="52"/>
+      <c r="BH3" s="52"/>
+      <c r="BI3" s="52"/>
+      <c r="BJ3" s="52"/>
+      <c r="BK3" s="52"/>
+      <c r="BL3" s="52"/>
+      <c r="BM3" s="52"/>
+      <c r="BN3" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="BO3" s="52"/>
-      <c r="BP3" s="52"/>
-      <c r="BQ3" s="52"/>
-      <c r="BR3" s="52"/>
-      <c r="BS3" s="52"/>
-      <c r="BT3" s="52"/>
-      <c r="BU3" s="52"/>
-      <c r="BV3" s="52"/>
-      <c r="BW3" s="52"/>
-      <c r="BX3" s="52"/>
-      <c r="BY3" s="52"/>
-      <c r="BZ3" s="52"/>
-      <c r="CA3" s="52"/>
-      <c r="CB3" s="52"/>
-      <c r="CC3" s="52"/>
-      <c r="CD3" s="52"/>
-      <c r="CE3" s="52"/>
-      <c r="CF3" s="52"/>
-      <c r="CG3" s="52"/>
-      <c r="CH3" s="52"/>
-      <c r="CI3" s="52"/>
-      <c r="CJ3" s="52"/>
-      <c r="CK3" s="52"/>
-      <c r="CL3" s="52"/>
-      <c r="CM3" s="52"/>
-      <c r="CN3" s="52"/>
-      <c r="CO3" s="52"/>
-      <c r="CP3" s="52"/>
-      <c r="CQ3" s="52"/>
-      <c r="CR3" s="52"/>
-      <c r="CS3" s="52" t="s">
+      <c r="BO3" s="53"/>
+      <c r="BP3" s="53"/>
+      <c r="BQ3" s="53"/>
+      <c r="BR3" s="53"/>
+      <c r="BS3" s="53"/>
+      <c r="BT3" s="53"/>
+      <c r="BU3" s="53"/>
+      <c r="BV3" s="53"/>
+      <c r="BW3" s="53"/>
+      <c r="BX3" s="53"/>
+      <c r="BY3" s="53"/>
+      <c r="BZ3" s="53"/>
+      <c r="CA3" s="53"/>
+      <c r="CB3" s="53"/>
+      <c r="CC3" s="53"/>
+      <c r="CD3" s="53"/>
+      <c r="CE3" s="53"/>
+      <c r="CF3" s="53"/>
+      <c r="CG3" s="53"/>
+      <c r="CH3" s="53"/>
+      <c r="CI3" s="53"/>
+      <c r="CJ3" s="53"/>
+      <c r="CK3" s="53"/>
+      <c r="CL3" s="53"/>
+      <c r="CM3" s="53"/>
+      <c r="CN3" s="53"/>
+      <c r="CO3" s="53"/>
+      <c r="CP3" s="53"/>
+      <c r="CQ3" s="53"/>
+      <c r="CR3" s="53"/>
+      <c r="CS3" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="CT3" s="52"/>
-      <c r="CU3" s="52"/>
-      <c r="CV3" s="52"/>
-      <c r="CW3" s="52"/>
-      <c r="CX3" s="52"/>
-      <c r="CY3" s="52"/>
-      <c r="CZ3" s="52"/>
-      <c r="DA3" s="52"/>
-      <c r="DB3" s="52"/>
-      <c r="DC3" s="52"/>
-      <c r="DD3" s="52"/>
-      <c r="DE3" s="52"/>
-      <c r="DF3" s="52"/>
-      <c r="DG3" s="52"/>
-      <c r="DH3" s="52"/>
-      <c r="DI3" s="52"/>
-      <c r="DJ3" s="52"/>
-      <c r="DK3" s="52"/>
-      <c r="DL3" s="52"/>
-      <c r="DM3" s="52"/>
-      <c r="DN3" s="52"/>
-      <c r="DO3" s="52"/>
-      <c r="DP3" s="52"/>
-      <c r="DQ3" s="52"/>
-      <c r="DR3" s="52"/>
-      <c r="DS3" s="52"/>
-      <c r="DT3" s="52"/>
+      <c r="CT3" s="53"/>
+      <c r="CU3" s="53"/>
+      <c r="CV3" s="53"/>
+      <c r="CW3" s="53"/>
+      <c r="CX3" s="53"/>
+      <c r="CY3" s="53"/>
+      <c r="CZ3" s="53"/>
+      <c r="DA3" s="53"/>
+      <c r="DB3" s="53"/>
+      <c r="DC3" s="53"/>
+      <c r="DD3" s="53"/>
+      <c r="DE3" s="53"/>
+      <c r="DF3" s="53"/>
+      <c r="DG3" s="53"/>
+      <c r="DH3" s="53"/>
+      <c r="DI3" s="53"/>
+      <c r="DJ3" s="53"/>
+      <c r="DK3" s="53"/>
+      <c r="DL3" s="53"/>
+      <c r="DM3" s="53"/>
+      <c r="DN3" s="53"/>
+      <c r="DO3" s="53"/>
+      <c r="DP3" s="53"/>
+      <c r="DQ3" s="53"/>
+      <c r="DR3" s="53"/>
+      <c r="DS3" s="53"/>
+      <c r="DT3" s="53"/>
     </row>
     <row r="4" spans="2:124" x14ac:dyDescent="0.25">
       <c r="C4" s="6">
@@ -2944,7 +2962,7 @@
       <c r="BL16" s="11"/>
       <c r="BM16" s="11"/>
     </row>
-    <row r="17" spans="2:67" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>203</v>
       </c>
@@ -2953,8 +2971,12 @@
       <c r="AY17" s="11"/>
       <c r="AZ17" s="11"/>
       <c r="BO17" s="11"/>
-    </row>
-    <row r="18" spans="2:67" x14ac:dyDescent="0.25">
+      <c r="BP17" s="11"/>
+      <c r="BV17" s="11"/>
+      <c r="BW17" s="11"/>
+      <c r="BZ17" s="11"/>
+    </row>
+    <row r="18" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>213</v>
       </c>
@@ -3058,11 +3080,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:BY39"/>
+  <dimension ref="A3:CD39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="BP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C18" sqref="C18"/>
+      <pane xSplit="3" topLeftCell="BR1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3086,25 +3108,26 @@
     <col min="69" max="69" width="11.7109375" customWidth="1"/>
     <col min="73" max="73" width="11.28515625" customWidth="1"/>
     <col min="75" max="75" width="18.5703125" customWidth="1"/>
+    <col min="82" max="82" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:77" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:82" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:82" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="62">
+      <c r="D4" s="63">
         <v>43523</v>
       </c>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="53">
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="54">
         <v>43524</v>
       </c>
-      <c r="H4" s="53"/>
+      <c r="H4" s="54"/>
       <c r="I4" s="7">
         <v>43525</v>
       </c>
@@ -3114,20 +3137,20 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="59">
+      <c r="L4" s="60">
         <v>43530</v>
       </c>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="53">
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="54">
         <v>43531</v>
       </c>
-      <c r="Q4" s="53"/>
-      <c r="R4" s="53">
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54">
         <v>43532</v>
       </c>
-      <c r="S4" s="53"/>
+      <c r="S4" s="54"/>
       <c r="T4" s="7">
         <v>43533</v>
       </c>
@@ -3146,55 +3169,55 @@
       <c r="Y4" s="7">
         <v>43539</v>
       </c>
-      <c r="Z4" s="53">
+      <c r="Z4" s="54">
         <v>43542</v>
       </c>
-      <c r="AA4" s="53"/>
-      <c r="AB4" s="53">
+      <c r="AA4" s="54"/>
+      <c r="AB4" s="54">
         <v>43543</v>
       </c>
-      <c r="AC4" s="53"/>
-      <c r="AD4" s="53"/>
+      <c r="AC4" s="54"/>
+      <c r="AD4" s="54"/>
       <c r="AE4" s="17">
         <v>43544</v>
       </c>
       <c r="AF4" s="18">
         <v>43545</v>
       </c>
-      <c r="AG4" s="53">
+      <c r="AG4" s="54">
         <v>43546</v>
       </c>
-      <c r="AH4" s="53"/>
+      <c r="AH4" s="54"/>
       <c r="AI4" s="35">
         <v>43547</v>
       </c>
-      <c r="AJ4" s="53">
+      <c r="AJ4" s="54">
         <v>43549</v>
       </c>
-      <c r="AK4" s="53"/>
-      <c r="AL4" s="53"/>
-      <c r="AM4" s="53"/>
-      <c r="AN4" s="53">
+      <c r="AK4" s="54"/>
+      <c r="AL4" s="54"/>
+      <c r="AM4" s="54"/>
+      <c r="AN4" s="54">
         <v>43550</v>
       </c>
-      <c r="AO4" s="53"/>
-      <c r="AP4" s="53"/>
-      <c r="AQ4" s="59">
+      <c r="AO4" s="54"/>
+      <c r="AP4" s="54"/>
+      <c r="AQ4" s="60">
         <v>43551</v>
       </c>
-      <c r="AR4" s="61"/>
+      <c r="AR4" s="62"/>
       <c r="AS4" s="7">
         <v>43552</v>
       </c>
-      <c r="AT4" s="53">
+      <c r="AT4" s="54">
         <v>43553</v>
       </c>
-      <c r="AU4" s="53"/>
-      <c r="AV4" s="53"/>
-      <c r="AW4" s="59">
+      <c r="AU4" s="54"/>
+      <c r="AV4" s="54"/>
+      <c r="AW4" s="60">
         <v>43556</v>
       </c>
-      <c r="AX4" s="61"/>
+      <c r="AX4" s="62"/>
       <c r="AY4" s="38">
         <v>43557</v>
       </c>
@@ -3204,40 +3227,40 @@
       <c r="BA4" s="7">
         <v>43559</v>
       </c>
-      <c r="BB4" s="53">
+      <c r="BB4" s="54">
         <v>43560</v>
       </c>
-      <c r="BC4" s="53"/>
+      <c r="BC4" s="54"/>
       <c r="BD4" s="39">
         <v>43563</v>
       </c>
-      <c r="BE4" s="53">
+      <c r="BE4" s="54">
         <v>43564</v>
       </c>
-      <c r="BF4" s="53"/>
-      <c r="BG4" s="53"/>
-      <c r="BH4" s="53">
+      <c r="BF4" s="54"/>
+      <c r="BG4" s="54"/>
+      <c r="BH4" s="54">
         <v>43565</v>
       </c>
-      <c r="BI4" s="53"/>
-      <c r="BJ4" s="53">
+      <c r="BI4" s="54"/>
+      <c r="BJ4" s="54">
         <v>43566</v>
       </c>
-      <c r="BK4" s="53"/>
-      <c r="BL4" s="53">
+      <c r="BK4" s="54"/>
+      <c r="BL4" s="54">
         <v>43567</v>
       </c>
-      <c r="BM4" s="53"/>
+      <c r="BM4" s="54"/>
       <c r="BN4" s="7">
         <v>43568</v>
       </c>
       <c r="BO4" s="7">
         <v>43570</v>
       </c>
-      <c r="BP4" s="53">
+      <c r="BP4" s="54">
         <v>43571</v>
       </c>
-      <c r="BQ4" s="53"/>
+      <c r="BQ4" s="54"/>
       <c r="BR4" s="42">
         <v>43572</v>
       </c>
@@ -3262,8 +3285,21 @@
       <c r="BY4" s="7">
         <v>43587</v>
       </c>
-    </row>
-    <row r="5" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BZ4" s="7">
+        <v>43588</v>
+      </c>
+      <c r="CA4" s="54">
+        <v>43594</v>
+      </c>
+      <c r="CB4" s="54"/>
+      <c r="CC4" s="46">
+        <v>43595</v>
+      </c>
+      <c r="CD4" s="7">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3285,7 +3321,7 @@
       <c r="BD5" s="40"/>
       <c r="BE5" s="40"/>
     </row>
-    <row r="6" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3299,7 +3335,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3313,7 +3349,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3327,41 +3363,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="57" t="s">
+      <c r="J9" s="58" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="55"/>
-      <c r="J10" s="58"/>
-    </row>
-    <row r="11" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="56"/>
+      <c r="J10" s="59"/>
+    </row>
+    <row r="11" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="56"/>
-      <c r="J11" s="58"/>
-    </row>
-    <row r="12" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="57"/>
+      <c r="J11" s="59"/>
+    </row>
+    <row r="12" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3375,7 +3411,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3407,7 +3443,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3442,7 +3478,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3474,7 +3510,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3602,7 +3638,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -3631,7 +3667,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -3639,21 +3675,39 @@
         <v>214</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="BY18" s="45" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="19" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BZ18" s="12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="20" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="CA19" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="CB19" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="CC19" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="CD19" s="45" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3661,7 +3715,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -3669,7 +3723,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3677,7 +3731,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -3685,7 +3739,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -3693,7 +3747,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -3701,7 +3755,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -3709,7 +3763,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -3717,15 +3771,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:77" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3734,11 +3788,13 @@
     <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
+    <mergeCell ref="CA4:CB4"/>
     <mergeCell ref="AW4:AX4"/>
     <mergeCell ref="AT4:AV4"/>
     <mergeCell ref="AN4:AP4"/>
     <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="BB4:BC4"/>
     <mergeCell ref="AJ4:AM4"/>
     <mergeCell ref="BL4:BM4"/>
     <mergeCell ref="BJ4:BK4"/>
@@ -3755,7 +3811,6 @@
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="BH4:BI4"/>
     <mergeCell ref="BE4:BG4"/>
-    <mergeCell ref="BB4:BC4"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A27">
     <cfRule type="colorScale" priority="8">

</xml_diff>

<commit_message>
preparacao para subir o aquifero alavanca inimigo atirador X
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="132" windowWidth="12828" windowHeight="8316" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="listaDeTarefasComEstimativas" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="224">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -684,7 +684,13 @@
     <t>21h30min-23h</t>
   </si>
   <si>
-    <t>8h30min</t>
+    <t>20h-22h</t>
+  </si>
+  <si>
+    <t>19h30min-23h30min</t>
+  </si>
+  <si>
+    <t>14h30min</t>
   </si>
 </sst>
 </file>
@@ -1535,13 +1541,13 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="44.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1596,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -1627,7 +1633,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>4</v>
       </c>
@@ -1655,7 +1661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>6</v>
       </c>
@@ -1692,7 +1698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>8</v>
       </c>
@@ -1772,7 +1778,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>15</v>
       </c>
@@ -1786,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>16</v>
       </c>
@@ -1794,7 +1800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>17</v>
       </c>
@@ -1808,7 +1814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>18</v>
       </c>
@@ -1816,7 +1822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>19</v>
       </c>
@@ -1824,7 +1830,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>20</v>
       </c>
@@ -1838,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>21</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>22</v>
       </c>
@@ -1866,7 +1872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>23</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>24</v>
       </c>
@@ -1888,7 +1894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
         <v>25</v>
       </c>
@@ -1896,7 +1902,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
         <v>26</v>
       </c>
@@ -1910,7 +1916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
         <v>27</v>
       </c>
@@ -1924,7 +1930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>28</v>
       </c>
@@ -1938,7 +1944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>29</v>
       </c>
@@ -1952,7 +1958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D35">
         <f>SUM(D5:D34)</f>
         <v>341</v>
@@ -1984,14 +1990,14 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="48.140625" customWidth="1"/>
-    <col min="5" max="5" width="41.140625" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="48.109375" customWidth="1"/>
+    <col min="5" max="5" width="41.109375" customWidth="1"/>
+    <col min="7" max="7" width="35.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0</v>
       </c>
@@ -2008,7 +2014,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -2025,7 +2031,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2</v>
       </c>
@@ -2042,7 +2048,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>3</v>
       </c>
@@ -2059,7 +2065,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>4</v>
       </c>
@@ -2076,7 +2082,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>5</v>
       </c>
@@ -2093,7 +2099,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>6</v>
       </c>
@@ -2110,7 +2116,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>7</v>
       </c>
@@ -2127,7 +2133,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>8</v>
       </c>
@@ -2144,7 +2150,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>9</v>
       </c>
@@ -2158,7 +2164,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>10</v>
       </c>
@@ -2172,7 +2178,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>11</v>
       </c>
@@ -2186,7 +2192,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>12</v>
       </c>
@@ -2194,7 +2200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>13</v>
       </c>
@@ -2202,7 +2208,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>14</v>
       </c>
@@ -2210,7 +2216,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>15</v>
       </c>
@@ -2218,7 +2224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>16</v>
       </c>
@@ -2226,7 +2232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>17</v>
       </c>
@@ -2234,7 +2240,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>18</v>
       </c>
@@ -2242,7 +2248,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>19</v>
       </c>
@@ -2250,7 +2256,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>20</v>
       </c>
@@ -2258,7 +2264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>21</v>
       </c>
@@ -2266,7 +2272,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>22</v>
       </c>
@@ -2274,7 +2280,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>23</v>
       </c>
@@ -2282,7 +2288,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>24</v>
       </c>
@@ -2290,7 +2296,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>25</v>
       </c>
@@ -2298,7 +2304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>26</v>
       </c>
@@ -2306,7 +2312,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>27</v>
       </c>
@@ -2314,7 +2320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>28</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>29</v>
       </c>
@@ -2339,19 +2345,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:DT18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AV1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="BZ17" sqref="BZ17"/>
+      <selection pane="topRight" activeCell="CA17" sqref="CA17:CB17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="44.42578125" customWidth="1"/>
-    <col min="3" max="124" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="44.44140625" customWidth="1"/>
+    <col min="3" max="124" width="5.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:124" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:124" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="50" t="s">
         <v>59</v>
       </c>
@@ -2485,7 +2491,7 @@
       <c r="DS3" s="53"/>
       <c r="DT3" s="53"/>
     </row>
-    <row r="4" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:124" ht="15" x14ac:dyDescent="0.25">
       <c r="C4" s="6">
         <v>27</v>
       </c>
@@ -2853,55 +2859,55 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:124" ht="15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="11"/>
     </row>
-    <row r="6" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:124" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:124" ht="15" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>68</v>
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:124" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>81</v>
       </c>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:124" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>69</v>
       </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:124" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>70</v>
       </c>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:124" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>74</v>
       </c>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:124" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>76</v>
       </c>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:124" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>71</v>
       </c>
@@ -2910,7 +2916,7 @@
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:124" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>96</v>
       </c>
@@ -2923,7 +2929,7 @@
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
     </row>
-    <row r="15" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:124" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>114</v>
       </c>
@@ -2933,7 +2939,7 @@
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
     </row>
-    <row r="16" spans="2:124" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:124" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>101</v>
       </c>
@@ -2962,7 +2968,7 @@
       <c r="BL16" s="11"/>
       <c r="BM16" s="11"/>
     </row>
-    <row r="17" spans="2:78" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:80" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>203</v>
       </c>
@@ -2975,8 +2981,10 @@
       <c r="BV17" s="11"/>
       <c r="BW17" s="11"/>
       <c r="BZ17" s="11"/>
-    </row>
-    <row r="18" spans="2:78" x14ac:dyDescent="0.25">
+      <c r="CA17" s="11"/>
+      <c r="CB17" s="11"/>
+    </row>
+    <row r="18" spans="2:80" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>213</v>
       </c>
@@ -3080,39 +3088,40 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:CD39"/>
+  <dimension ref="A3:CF39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" topLeftCell="BR1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="48" width="17.85546875" customWidth="1"/>
-    <col min="49" max="50" width="12.5703125" customWidth="1"/>
-    <col min="51" max="51" width="10.5703125" customWidth="1"/>
-    <col min="52" max="52" width="19.85546875" customWidth="1"/>
-    <col min="54" max="54" width="18.85546875" customWidth="1"/>
-    <col min="55" max="55" width="19.5703125" customWidth="1"/>
-    <col min="56" max="59" width="18.42578125" customWidth="1"/>
-    <col min="60" max="60" width="18.5703125" customWidth="1"/>
-    <col min="61" max="61" width="17.5703125" customWidth="1"/>
-    <col min="62" max="63" width="17.85546875" customWidth="1"/>
-    <col min="64" max="64" width="18.5703125" customWidth="1"/>
-    <col min="65" max="65" width="14.85546875" customWidth="1"/>
-    <col min="66" max="66" width="13.7109375" customWidth="1"/>
-    <col min="68" max="68" width="18.140625" customWidth="1"/>
-    <col min="69" max="69" width="11.7109375" customWidth="1"/>
-    <col min="73" max="73" width="11.28515625" customWidth="1"/>
-    <col min="75" max="75" width="18.5703125" customWidth="1"/>
-    <col min="82" max="82" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="48" width="17.88671875" customWidth="1"/>
+    <col min="49" max="50" width="12.5546875" customWidth="1"/>
+    <col min="51" max="51" width="10.5546875" customWidth="1"/>
+    <col min="52" max="52" width="19.88671875" customWidth="1"/>
+    <col min="54" max="54" width="18.88671875" customWidth="1"/>
+    <col min="55" max="55" width="19.5546875" customWidth="1"/>
+    <col min="56" max="59" width="18.44140625" customWidth="1"/>
+    <col min="60" max="60" width="18.5546875" customWidth="1"/>
+    <col min="61" max="61" width="17.5546875" customWidth="1"/>
+    <col min="62" max="63" width="17.88671875" customWidth="1"/>
+    <col min="64" max="64" width="18.5546875" customWidth="1"/>
+    <col min="65" max="65" width="14.88671875" customWidth="1"/>
+    <col min="66" max="66" width="13.6640625" customWidth="1"/>
+    <col min="68" max="68" width="18.109375" customWidth="1"/>
+    <col min="69" max="69" width="11.6640625" customWidth="1"/>
+    <col min="73" max="73" width="11.33203125" customWidth="1"/>
+    <col min="75" max="75" width="18.5546875" customWidth="1"/>
+    <col min="82" max="82" width="13.88671875" customWidth="1"/>
+    <col min="84" max="84" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:82" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:82" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:84" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
@@ -3298,8 +3307,14 @@
       <c r="CD4" s="7">
         <v>43598</v>
       </c>
-    </row>
-    <row r="5" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CE4" s="7">
+        <v>43599</v>
+      </c>
+      <c r="CF4" s="7">
+        <v>43600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3321,7 +3336,7 @@
       <c r="BD5" s="40"/>
       <c r="BE5" s="40"/>
     </row>
-    <row r="6" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3335,7 +3350,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3349,7 +3364,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3363,7 +3378,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3377,7 +3392,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3387,7 +3402,7 @@
       <c r="C10" s="56"/>
       <c r="J10" s="59"/>
     </row>
-    <row r="11" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -3397,7 +3412,7 @@
       <c r="C11" s="57"/>
       <c r="J11" s="59"/>
     </row>
-    <row r="12" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3411,7 +3426,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3443,7 +3458,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3478,7 +3493,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3510,7 +3525,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3638,7 +3653,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
@@ -3667,7 +3682,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
@@ -3684,7 +3699,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15</v>
       </c>
@@ -3692,7 +3707,7 @@
         <v>102</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="CA19" s="11" t="s">
         <v>216</v>
@@ -3706,8 +3721,14 @@
       <c r="CD19" s="45" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="20" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CE19" s="45" t="s">
+        <v>221</v>
+      </c>
+      <c r="CF19" s="45" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="20" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3715,7 +3736,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17</v>
       </c>
@@ -3723,7 +3744,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3731,7 +3752,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>19</v>
       </c>
@@ -3739,7 +3760,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20</v>
       </c>
@@ -3747,7 +3768,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>21</v>
       </c>
@@ -3755,7 +3776,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>22</v>
       </c>
@@ -3763,7 +3784,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>23</v>
       </c>
@@ -3771,22 +3792,22 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:82" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="22">
     <mergeCell ref="CA4:CB4"/>
@@ -3849,20 +3870,20 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="7" max="7" width="29.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="7" max="7" width="29.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="19" t="s">
         <v>122</v>
       </c>
@@ -3885,7 +3906,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="135.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" ht="115.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B5" s="21" t="s">
         <v>124</v>
       </c>
@@ -3908,7 +3929,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B6" s="21" t="s">
         <v>133</v>
       </c>
@@ -3931,7 +3952,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B7" s="21" t="s">
         <v>139</v>
       </c>
@@ -3960,7 +3981,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B8" s="21" t="s">
         <v>147</v>
       </c>
@@ -3986,7 +4007,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" ht="144" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
         <v>153</v>
       </c>
@@ -4029,10 +4050,10 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="38.85546875" customWidth="1"/>
-    <col min="4" max="7" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" customWidth="1"/>
+    <col min="4" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4134,7 +4155,7 @@
       <c r="F13" s="33"/>
       <c r="G13" s="34"/>
     </row>
-    <row r="14" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="32" t="s">
         <v>170</v>
       </c>
@@ -4152,7 +4173,7 @@
       <c r="F15" s="33"/>
       <c r="G15" s="34"/>
     </row>
-    <row r="16" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="32" t="s">
         <v>172</v>
       </c>
@@ -4161,7 +4182,7 @@
       <c r="F16" s="33"/>
       <c r="G16" s="34"/>
     </row>
-    <row r="17" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="32" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
subida do aquifero checkpoint do aquifero inicio do desafio dos xshooters
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="132" windowWidth="12828" windowHeight="8316" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="listaDeTarefasComEstimativas" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="224">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -690,7 +690,7 @@
     <t>19h30min-23h30min</t>
   </si>
   <si>
-    <t>14h30min</t>
+    <t>16h30min</t>
   </si>
 </sst>
 </file>
@@ -1187,6 +1187,12 @@
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1202,13 +1208,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1541,13 +1541,13 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="44.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1602,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>43511</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>4</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>6</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>8</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>15</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>16</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>17</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>18</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>19</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>20</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>21</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>22</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>23</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>24</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>25</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>26</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>27</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>28</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>29</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D35">
         <f>SUM(D5:D34)</f>
         <v>341</v>
@@ -1990,14 +1990,14 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="48.109375" customWidth="1"/>
-    <col min="5" max="5" width="41.109375" customWidth="1"/>
-    <col min="7" max="7" width="35.88671875" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>3</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>4</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>5</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>6</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>7</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>8</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>9</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>10</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>11</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>12</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>13</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>14</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>15</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>16</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>17</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>18</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>19</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>20</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>21</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>22</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>23</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>24</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>25</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>26</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>27</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>28</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>29</v>
       </c>
@@ -2345,19 +2345,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:DT18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="AV1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="CA17" sqref="CA17:CB17"/>
+      <selection pane="topRight" activeCell="CC17" sqref="CC17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="44.44140625" customWidth="1"/>
-    <col min="3" max="124" width="5.44140625" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="124" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:124" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:124" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="50" t="s">
         <v>59</v>
       </c>
@@ -2491,7 +2491,7 @@
       <c r="DS3" s="53"/>
       <c r="DT3" s="53"/>
     </row>
-    <row r="4" spans="2:124" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:124" x14ac:dyDescent="0.25">
       <c r="C4" s="6">
         <v>27</v>
       </c>
@@ -2859,55 +2859,55 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="2:124" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="11"/>
     </row>
-    <row r="6" spans="2:124" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="2:124" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>68</v>
       </c>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="2:124" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>81</v>
       </c>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="2:124" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>69</v>
       </c>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" spans="2:124" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>70</v>
       </c>
       <c r="H10" s="11"/>
     </row>
-    <row r="11" spans="2:124" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>74</v>
       </c>
       <c r="H11" s="11"/>
     </row>
-    <row r="12" spans="2:124" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>76</v>
       </c>
       <c r="H12" s="11"/>
     </row>
-    <row r="13" spans="2:124" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>71</v>
       </c>
@@ -2916,7 +2916,7 @@
       <c r="K13" s="11"/>
       <c r="L13" s="11"/>
     </row>
-    <row r="14" spans="2:124" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>96</v>
       </c>
@@ -2929,7 +2929,7 @@
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
     </row>
-    <row r="15" spans="2:124" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>114</v>
       </c>
@@ -2939,7 +2939,7 @@
       <c r="W15" s="11"/>
       <c r="X15" s="11"/>
     </row>
-    <row r="16" spans="2:124" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:124" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>101</v>
       </c>
@@ -2968,7 +2968,7 @@
       <c r="BL16" s="11"/>
       <c r="BM16" s="11"/>
     </row>
-    <row r="17" spans="2:80" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:81" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>203</v>
       </c>
@@ -2983,8 +2983,9 @@
       <c r="BZ17" s="11"/>
       <c r="CA17" s="11"/>
       <c r="CB17" s="11"/>
-    </row>
-    <row r="18" spans="2:80" x14ac:dyDescent="0.3">
+      <c r="CC17" s="11"/>
+    </row>
+    <row r="18" spans="2:81" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>213</v>
       </c>
@@ -3088,40 +3089,40 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:CF39"/>
+  <dimension ref="A3:CG39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" topLeftCell="BR1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C20" sqref="C20"/>
+      <selection pane="topRight" activeCell="CG4" sqref="CG4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="48" width="17.88671875" customWidth="1"/>
-    <col min="49" max="50" width="12.5546875" customWidth="1"/>
-    <col min="51" max="51" width="10.5546875" customWidth="1"/>
-    <col min="52" max="52" width="19.88671875" customWidth="1"/>
-    <col min="54" max="54" width="18.88671875" customWidth="1"/>
-    <col min="55" max="55" width="19.5546875" customWidth="1"/>
-    <col min="56" max="59" width="18.44140625" customWidth="1"/>
-    <col min="60" max="60" width="18.5546875" customWidth="1"/>
-    <col min="61" max="61" width="17.5546875" customWidth="1"/>
-    <col min="62" max="63" width="17.88671875" customWidth="1"/>
-    <col min="64" max="64" width="18.5546875" customWidth="1"/>
-    <col min="65" max="65" width="14.88671875" customWidth="1"/>
-    <col min="66" max="66" width="13.6640625" customWidth="1"/>
-    <col min="68" max="68" width="18.109375" customWidth="1"/>
-    <col min="69" max="69" width="11.6640625" customWidth="1"/>
-    <col min="73" max="73" width="11.33203125" customWidth="1"/>
-    <col min="75" max="75" width="18.5546875" customWidth="1"/>
-    <col min="82" max="82" width="13.88671875" customWidth="1"/>
-    <col min="84" max="84" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="48" width="17.85546875" customWidth="1"/>
+    <col min="49" max="50" width="12.5703125" customWidth="1"/>
+    <col min="51" max="51" width="10.5703125" customWidth="1"/>
+    <col min="52" max="52" width="19.85546875" customWidth="1"/>
+    <col min="54" max="54" width="18.85546875" customWidth="1"/>
+    <col min="55" max="55" width="19.5703125" customWidth="1"/>
+    <col min="56" max="59" width="18.42578125" customWidth="1"/>
+    <col min="60" max="60" width="18.5703125" customWidth="1"/>
+    <col min="61" max="61" width="17.5703125" customWidth="1"/>
+    <col min="62" max="63" width="17.85546875" customWidth="1"/>
+    <col min="64" max="64" width="18.5703125" customWidth="1"/>
+    <col min="65" max="65" width="14.85546875" customWidth="1"/>
+    <col min="66" max="66" width="13.7109375" customWidth="1"/>
+    <col min="68" max="68" width="18.140625" customWidth="1"/>
+    <col min="69" max="69" width="11.7109375" customWidth="1"/>
+    <col min="73" max="73" width="11.28515625" customWidth="1"/>
+    <col min="75" max="75" width="18.5703125" customWidth="1"/>
+    <col min="82" max="82" width="13.85546875" customWidth="1"/>
+    <col min="84" max="84" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:84" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:84" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:85" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
@@ -3146,12 +3147,12 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="60">
+      <c r="L4" s="55">
         <v>43530</v>
       </c>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="56"/>
       <c r="P4" s="54">
         <v>43531</v>
       </c>
@@ -3211,10 +3212,10 @@
       </c>
       <c r="AO4" s="54"/>
       <c r="AP4" s="54"/>
-      <c r="AQ4" s="60">
+      <c r="AQ4" s="55">
         <v>43551</v>
       </c>
-      <c r="AR4" s="62"/>
+      <c r="AR4" s="56"/>
       <c r="AS4" s="7">
         <v>43552</v>
       </c>
@@ -3223,10 +3224,10 @@
       </c>
       <c r="AU4" s="54"/>
       <c r="AV4" s="54"/>
-      <c r="AW4" s="60">
+      <c r="AW4" s="55">
         <v>43556</v>
       </c>
-      <c r="AX4" s="62"/>
+      <c r="AX4" s="56"/>
       <c r="AY4" s="38">
         <v>43557</v>
       </c>
@@ -3313,8 +3314,11 @@
       <c r="CF4" s="7">
         <v>43600</v>
       </c>
-    </row>
-    <row r="5" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CG4" s="7">
+        <v>43601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3336,7 +3340,7 @@
       <c r="BD5" s="40"/>
       <c r="BE5" s="40"/>
     </row>
-    <row r="6" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3350,7 +3354,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3364,7 +3368,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3378,41 +3382,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="58" t="s">
+      <c r="J9" s="60" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="J10" s="59"/>
-    </row>
-    <row r="11" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="58"/>
+      <c r="J10" s="61"/>
+    </row>
+    <row r="11" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="J11" s="59"/>
-    </row>
-    <row r="12" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="59"/>
+      <c r="J11" s="61"/>
+    </row>
+    <row r="12" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3426,7 +3430,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3458,7 +3462,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3493,7 +3497,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3525,7 +3529,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3653,7 +3657,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -3682,7 +3686,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -3699,7 +3703,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -3727,8 +3731,11 @@
       <c r="CF19" s="45" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="20" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="CG19" s="45" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3736,7 +3743,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -3744,7 +3751,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3752,7 +3759,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -3760,7 +3767,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -3768,7 +3775,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -3776,7 +3783,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -3784,7 +3791,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -3792,30 +3799,24 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:84" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="CA4:CB4"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="BB4:BC4"/>
     <mergeCell ref="AJ4:AM4"/>
     <mergeCell ref="BL4:BM4"/>
     <mergeCell ref="BJ4:BK4"/>
@@ -3832,6 +3833,12 @@
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="BH4:BI4"/>
     <mergeCell ref="BE4:BG4"/>
+    <mergeCell ref="CA4:CB4"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="BB4:BC4"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A27">
     <cfRule type="colorScale" priority="8">
@@ -3870,20 +3877,20 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" customWidth="1"/>
-    <col min="7" max="7" width="29.109375" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
         <v>122</v>
       </c>
@@ -3906,7 +3913,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="115.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="135.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
         <v>124</v>
       </c>
@@ -3929,7 +3936,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="105" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
         <v>133</v>
       </c>
@@ -3952,7 +3959,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="150" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
         <v>139</v>
       </c>
@@ -3981,7 +3988,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="120" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
         <v>147</v>
       </c>
@@ -4007,7 +4014,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="144" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="150" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
         <v>153</v>
       </c>
@@ -4050,10 +4057,10 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.88671875" customWidth="1"/>
-    <col min="4" max="7" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4155,7 +4162,7 @@
       <c r="F13" s="33"/>
       <c r="G13" s="34"/>
     </row>
-    <row r="14" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="32" t="s">
         <v>170</v>
       </c>
@@ -4173,7 +4180,7 @@
       <c r="F15" s="33"/>
       <c r="G15" s="34"/>
     </row>
-    <row r="16" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="32" t="s">
         <v>172</v>
       </c>
@@ -4182,7 +4189,7 @@
       <c r="F16" s="33"/>
       <c r="G16" s="34"/>
     </row>
-    <row r="17" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="32" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
em meio a capsula do aquifero
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="listaDeTarefasComEstimativas" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="233">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -690,7 +690,34 @@
     <t>19h30min-23h30min</t>
   </si>
   <si>
-    <t>16h30min</t>
+    <t>12h-14h30min</t>
+  </si>
+  <si>
+    <t>19h30min - 22h</t>
+  </si>
+  <si>
+    <t>9h-12h</t>
+  </si>
+  <si>
+    <t>21h30min-0h</t>
+  </si>
+  <si>
+    <t>19h-23h</t>
+  </si>
+  <si>
+    <t>19h-21h30min</t>
+  </si>
+  <si>
+    <t>Área 2</t>
+  </si>
+  <si>
+    <t>13h30min-15h</t>
+  </si>
+  <si>
+    <t>9h-12</t>
+  </si>
+  <si>
+    <t>45h30min</t>
   </si>
 </sst>
 </file>
@@ -1187,12 +1214,6 @@
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1208,7 +1229,13 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2343,12 +2370,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:DT18"/>
+  <dimension ref="B3:DT19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AV1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="CC17" sqref="CC17"/>
+      <selection pane="topRight" activeCell="CK19" sqref="CK19:CL19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2968,7 +2995,7 @@
       <c r="BL16" s="11"/>
       <c r="BM16" s="11"/>
     </row>
-    <row r="17" spans="2:81" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>203</v>
       </c>
@@ -2976,19 +3003,31 @@
       <c r="AX17" s="11"/>
       <c r="AY17" s="11"/>
       <c r="AZ17" s="11"/>
-      <c r="BO17" s="11"/>
-      <c r="BP17" s="11"/>
-      <c r="BV17" s="11"/>
-      <c r="BW17" s="11"/>
-      <c r="BZ17" s="11"/>
-      <c r="CA17" s="11"/>
-      <c r="CB17" s="11"/>
-      <c r="CC17" s="11"/>
-    </row>
-    <row r="18" spans="2:81" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:90" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>213</v>
       </c>
+      <c r="BO18" s="11"/>
+      <c r="BP18" s="11"/>
+    </row>
+    <row r="19" spans="2:90" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>229</v>
+      </c>
+      <c r="BV19" s="11"/>
+      <c r="BW19" s="11"/>
+      <c r="BZ19" s="11"/>
+      <c r="CA19" s="11"/>
+      <c r="CB19" s="11"/>
+      <c r="CC19" s="11"/>
+      <c r="CD19" s="11"/>
+      <c r="CE19" s="11"/>
+      <c r="CH19" s="11"/>
+      <c r="CI19" s="11"/>
+      <c r="CJ19" s="11"/>
+      <c r="CK19" s="11"/>
+      <c r="CL19" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3089,11 +3128,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:CG39"/>
+  <dimension ref="A3:CR39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="BR1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CG4" sqref="CG4"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" topLeftCell="CC1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3119,10 +3158,17 @@
     <col min="75" max="75" width="18.5703125" customWidth="1"/>
     <col min="82" max="82" width="13.85546875" customWidth="1"/>
     <col min="84" max="84" width="17.85546875" customWidth="1"/>
+    <col min="85" max="85" width="9.140625" customWidth="1"/>
+    <col min="86" max="86" width="13.85546875" customWidth="1"/>
+    <col min="87" max="87" width="14.5703125" customWidth="1"/>
+    <col min="89" max="89" width="12.5703125" customWidth="1"/>
+    <col min="90" max="90" width="18.42578125" customWidth="1"/>
+    <col min="93" max="93" width="13.28515625" customWidth="1"/>
+    <col min="94" max="95" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:85" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:96" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:96" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
@@ -3147,12 +3193,12 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="55">
+      <c r="L4" s="60">
         <v>43530</v>
       </c>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="56"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="62"/>
       <c r="P4" s="54">
         <v>43531</v>
       </c>
@@ -3212,10 +3258,10 @@
       </c>
       <c r="AO4" s="54"/>
       <c r="AP4" s="54"/>
-      <c r="AQ4" s="55">
+      <c r="AQ4" s="60">
         <v>43551</v>
       </c>
-      <c r="AR4" s="56"/>
+      <c r="AR4" s="62"/>
       <c r="AS4" s="7">
         <v>43552</v>
       </c>
@@ -3224,10 +3270,10 @@
       </c>
       <c r="AU4" s="54"/>
       <c r="AV4" s="54"/>
-      <c r="AW4" s="55">
+      <c r="AW4" s="60">
         <v>43556</v>
       </c>
-      <c r="AX4" s="56"/>
+      <c r="AX4" s="62"/>
       <c r="AY4" s="38">
         <v>43557</v>
       </c>
@@ -3317,8 +3363,33 @@
       <c r="CG4" s="7">
         <v>43601</v>
       </c>
-    </row>
-    <row r="5" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH4" s="54">
+        <v>43602</v>
+      </c>
+      <c r="CI4" s="54"/>
+      <c r="CJ4" s="7">
+        <v>43603</v>
+      </c>
+      <c r="CK4" s="7">
+        <v>43605</v>
+      </c>
+      <c r="CL4" s="54">
+        <v>43607</v>
+      </c>
+      <c r="CM4" s="54"/>
+      <c r="CN4" s="54">
+        <v>43608</v>
+      </c>
+      <c r="CO4" s="54"/>
+      <c r="CP4" s="54">
+        <v>43609</v>
+      </c>
+      <c r="CQ4" s="54"/>
+      <c r="CR4" s="7">
+        <v>43610</v>
+      </c>
+    </row>
+    <row r="5" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3340,7 +3411,7 @@
       <c r="BD5" s="40"/>
       <c r="BE5" s="40"/>
     </row>
-    <row r="6" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3354,7 +3425,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3368,7 +3439,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3382,41 +3453,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="58" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="J10" s="61"/>
-    </row>
-    <row r="11" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="56"/>
+      <c r="J10" s="59"/>
+    </row>
+    <row r="11" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="59"/>
-      <c r="J11" s="61"/>
-    </row>
-    <row r="12" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="57"/>
+      <c r="J11" s="59"/>
+    </row>
+    <row r="12" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3430,7 +3501,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3462,7 +3533,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3497,7 +3568,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3529,7 +3600,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3657,7 +3728,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -3686,7 +3757,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -3703,7 +3774,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -3711,7 +3782,7 @@
         <v>102</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="CA19" s="11" t="s">
         <v>216</v>
@@ -3734,8 +3805,41 @@
       <c r="CG19" s="45" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="20" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CH19" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="CI19" s="45" t="s">
+        <v>224</v>
+      </c>
+      <c r="CJ19" s="45" t="s">
+        <v>225</v>
+      </c>
+      <c r="CK19" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="CL19" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="CM19" s="45" t="s">
+        <v>227</v>
+      </c>
+      <c r="CN19" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="CO19" s="45" t="s">
+        <v>228</v>
+      </c>
+      <c r="CP19" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="CQ19" s="45" t="s">
+        <v>230</v>
+      </c>
+      <c r="CR19" s="45" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3743,7 +3847,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -3751,7 +3855,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3759,7 +3863,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -3767,7 +3871,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -3775,7 +3879,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -3783,7 +3887,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -3791,7 +3895,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -3799,15 +3903,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:85" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3816,11 +3920,18 @@
     <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="AJ4:AM4"/>
-    <mergeCell ref="BL4:BM4"/>
-    <mergeCell ref="BJ4:BK4"/>
-    <mergeCell ref="BP4:BQ4"/>
+  <mergeCells count="26">
+    <mergeCell ref="CP4:CQ4"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="BH4:BI4"/>
+    <mergeCell ref="BE4:BG4"/>
+    <mergeCell ref="CH4:CI4"/>
+    <mergeCell ref="CA4:CB4"/>
+    <mergeCell ref="AW4:AX4"/>
+    <mergeCell ref="AT4:AV4"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="AQ4:AR4"/>
+    <mergeCell ref="BB4:BC4"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="L4:O4"/>
@@ -3830,15 +3941,12 @@
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="BH4:BI4"/>
-    <mergeCell ref="BE4:BG4"/>
-    <mergeCell ref="CA4:CB4"/>
-    <mergeCell ref="AW4:AX4"/>
-    <mergeCell ref="AT4:AV4"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="AQ4:AR4"/>
-    <mergeCell ref="BB4:BC4"/>
+    <mergeCell ref="CL4:CM4"/>
+    <mergeCell ref="CN4:CO4"/>
+    <mergeCell ref="AJ4:AM4"/>
+    <mergeCell ref="BL4:BM4"/>
+    <mergeCell ref="BJ4:BK4"/>
+    <mergeCell ref="BP4:BQ4"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A27">
     <cfRule type="colorScale" priority="8">

</xml_diff>

<commit_message>
seta sombria gameplay implementado
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="listaDeTarefasComEstimativas" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="234">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -717,7 +717,10 @@
     <t>9h-12</t>
   </si>
   <si>
-    <t>45h30min</t>
+    <t>19h30min-23h</t>
+  </si>
+  <si>
+    <t>49h</t>
   </si>
 </sst>
 </file>
@@ -1214,6 +1217,12 @@
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1229,13 +1238,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2372,10 +2375,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:DT19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="BJ1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="CK19" sqref="CK19:CL19"/>
+      <selection pane="topRight" activeCell="CO19" sqref="CO19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2995,7 +2998,7 @@
       <c r="BL16" s="11"/>
       <c r="BM16" s="11"/>
     </row>
-    <row r="17" spans="2:90" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:93" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>203</v>
       </c>
@@ -3004,14 +3007,14 @@
       <c r="AY17" s="11"/>
       <c r="AZ17" s="11"/>
     </row>
-    <row r="18" spans="2:90" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:93" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>213</v>
       </c>
       <c r="BO18" s="11"/>
       <c r="BP18" s="11"/>
     </row>
-    <row r="19" spans="2:90" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:93" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>229</v>
       </c>
@@ -3028,6 +3031,7 @@
       <c r="CJ19" s="11"/>
       <c r="CK19" s="11"/>
       <c r="CL19" s="11"/>
+      <c r="CO19" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3128,10 +3132,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:CR39"/>
+  <dimension ref="A3:CS39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="CC1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="CH1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -3165,10 +3169,11 @@
     <col min="90" max="90" width="18.42578125" customWidth="1"/>
     <col min="93" max="93" width="13.28515625" customWidth="1"/>
     <col min="94" max="95" width="13" customWidth="1"/>
+    <col min="97" max="97" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:96" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:96" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:97" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:97" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
@@ -3193,12 +3198,12 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="60">
+      <c r="L4" s="55">
         <v>43530</v>
       </c>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="56"/>
       <c r="P4" s="54">
         <v>43531</v>
       </c>
@@ -3258,10 +3263,10 @@
       </c>
       <c r="AO4" s="54"/>
       <c r="AP4" s="54"/>
-      <c r="AQ4" s="60">
+      <c r="AQ4" s="55">
         <v>43551</v>
       </c>
-      <c r="AR4" s="62"/>
+      <c r="AR4" s="56"/>
       <c r="AS4" s="7">
         <v>43552</v>
       </c>
@@ -3270,10 +3275,10 @@
       </c>
       <c r="AU4" s="54"/>
       <c r="AV4" s="54"/>
-      <c r="AW4" s="60">
+      <c r="AW4" s="55">
         <v>43556</v>
       </c>
-      <c r="AX4" s="62"/>
+      <c r="AX4" s="56"/>
       <c r="AY4" s="38">
         <v>43557</v>
       </c>
@@ -3388,8 +3393,11 @@
       <c r="CR4" s="7">
         <v>43610</v>
       </c>
-    </row>
-    <row r="5" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CS4" s="7">
+        <v>43613</v>
+      </c>
+    </row>
+    <row r="5" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3411,7 +3419,7 @@
       <c r="BD5" s="40"/>
       <c r="BE5" s="40"/>
     </row>
-    <row r="6" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3425,7 +3433,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3439,7 +3447,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3453,41 +3461,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="58" t="s">
+      <c r="J9" s="60" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="J10" s="59"/>
-    </row>
-    <row r="11" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="58"/>
+      <c r="J10" s="61"/>
+    </row>
+    <row r="11" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="J11" s="59"/>
-    </row>
-    <row r="12" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="59"/>
+      <c r="J11" s="61"/>
+    </row>
+    <row r="12" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3501,7 +3509,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3533,7 +3541,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3568,7 +3576,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3600,7 +3608,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3728,7 +3736,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -3757,7 +3765,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -3774,7 +3782,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -3782,7 +3790,7 @@
         <v>102</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="CA19" s="11" t="s">
         <v>216</v>
@@ -3838,8 +3846,11 @@
       <c r="CR19" s="45" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="20" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CS19" s="45" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="20" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3847,7 +3858,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -3855,7 +3866,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3863,7 +3874,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -3871,7 +3882,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -3879,7 +3890,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -3887,7 +3898,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -3895,7 +3906,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -3903,15 +3914,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:96" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3921,6 +3932,16 @@
     <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="BP4:BQ4"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
     <mergeCell ref="CP4:CQ4"/>
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="BH4:BI4"/>
@@ -3932,21 +3953,11 @@
     <mergeCell ref="AN4:AP4"/>
     <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="BB4:BC4"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:H4"/>
     <mergeCell ref="CL4:CM4"/>
     <mergeCell ref="CN4:CO4"/>
     <mergeCell ref="AJ4:AM4"/>
     <mergeCell ref="BL4:BM4"/>
     <mergeCell ref="BJ4:BK4"/>
-    <mergeCell ref="BP4:BQ4"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A27">
     <cfRule type="colorScale" priority="8">

</xml_diff>

<commit_message>
iniciando pos chefe seta sombria
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="236">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -720,7 +720,13 @@
     <t>19h30min-23h</t>
   </si>
   <si>
-    <t>49h</t>
+    <t>13h30min-15h30min</t>
+  </si>
+  <si>
+    <t>13h-16</t>
+  </si>
+  <si>
+    <t>60h</t>
   </si>
 </sst>
 </file>
@@ -1217,12 +1223,6 @@
     <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1238,7 +1238,13 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3132,10 +3138,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:CS39"/>
+  <dimension ref="A3:CX39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="CH1" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" topLeftCell="CI1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -3170,10 +3176,13 @@
     <col min="93" max="93" width="13.28515625" customWidth="1"/>
     <col min="94" max="95" width="13" customWidth="1"/>
     <col min="97" max="97" width="14" customWidth="1"/>
+    <col min="98" max="98" width="20" customWidth="1"/>
+    <col min="99" max="99" width="20.42578125" customWidth="1"/>
+    <col min="101" max="101" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:97" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:97" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:102" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:102" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
@@ -3198,12 +3207,12 @@
       <c r="K4" s="7">
         <v>43529</v>
       </c>
-      <c r="L4" s="55">
+      <c r="L4" s="60">
         <v>43530</v>
       </c>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="56"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="62"/>
       <c r="P4" s="54">
         <v>43531</v>
       </c>
@@ -3263,10 +3272,10 @@
       </c>
       <c r="AO4" s="54"/>
       <c r="AP4" s="54"/>
-      <c r="AQ4" s="55">
+      <c r="AQ4" s="60">
         <v>43551</v>
       </c>
-      <c r="AR4" s="56"/>
+      <c r="AR4" s="62"/>
       <c r="AS4" s="7">
         <v>43552</v>
       </c>
@@ -3275,10 +3284,10 @@
       </c>
       <c r="AU4" s="54"/>
       <c r="AV4" s="54"/>
-      <c r="AW4" s="55">
+      <c r="AW4" s="60">
         <v>43556</v>
       </c>
-      <c r="AX4" s="56"/>
+      <c r="AX4" s="62"/>
       <c r="AY4" s="38">
         <v>43557</v>
       </c>
@@ -3396,8 +3405,19 @@
       <c r="CS4" s="7">
         <v>43613</v>
       </c>
-    </row>
-    <row r="5" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CT4" s="54">
+        <v>43616</v>
+      </c>
+      <c r="CU4" s="54"/>
+      <c r="CV4" s="7">
+        <v>43619</v>
+      </c>
+      <c r="CW4" s="54">
+        <v>43621</v>
+      </c>
+      <c r="CX4" s="54"/>
+    </row>
+    <row r="5" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3419,7 +3439,7 @@
       <c r="BD5" s="40"/>
       <c r="BE5" s="40"/>
     </row>
-    <row r="6" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3433,7 +3453,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3447,7 +3467,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3461,41 +3481,41 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="58" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="J10" s="61"/>
-    </row>
-    <row r="11" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="56"/>
+      <c r="J10" s="59"/>
+    </row>
+    <row r="11" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="59"/>
-      <c r="J11" s="61"/>
-    </row>
-    <row r="12" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="57"/>
+      <c r="J11" s="59"/>
+    </row>
+    <row r="12" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3509,7 +3529,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3541,7 +3561,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3576,7 +3596,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3608,7 +3628,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3736,7 +3756,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -3765,7 +3785,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -3782,7 +3802,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -3790,7 +3810,7 @@
         <v>102</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="CA19" s="11" t="s">
         <v>216</v>
@@ -3849,8 +3869,23 @@
       <c r="CS19" s="45" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="20" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CT19" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="CU19" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="CV19" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="CW19" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="CX19" s="45" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3858,7 +3893,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -3866,7 +3901,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3874,7 +3909,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -3882,7 +3917,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -3890,7 +3925,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -3898,7 +3933,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -3906,7 +3941,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -3914,15 +3949,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:97" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:102" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3931,17 +3966,9 @@
     <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="BP4:BQ4"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="J9:J11"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="G4:H4"/>
+  <mergeCells count="28">
+    <mergeCell ref="CT4:CU4"/>
+    <mergeCell ref="CW4:CX4"/>
     <mergeCell ref="CP4:CQ4"/>
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="BH4:BI4"/>
@@ -3958,6 +3985,16 @@
     <mergeCell ref="AJ4:AM4"/>
     <mergeCell ref="BL4:BM4"/>
     <mergeCell ref="BJ4:BK4"/>
+    <mergeCell ref="BP4:BQ4"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A27">
     <cfRule type="colorScale" priority="8">

</xml_diff>

<commit_message>
fazendo o text language converter
</commit_message>
<xml_diff>
--- a/Assets/Documents/planejamento.xlsx
+++ b/Assets/Documents/planejamento.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="12825" windowHeight="8310" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="listaDeTarefasComEstimativas" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="239">
   <si>
     <t>Definir o escopo</t>
   </si>
@@ -729,7 +729,13 @@
     <t>13h-17h</t>
   </si>
   <si>
-    <t>66h</t>
+    <t>10h30min - 11h</t>
+  </si>
+  <si>
+    <t>12h-15h</t>
+  </si>
+  <si>
+    <t>80h30min</t>
   </si>
 </sst>
 </file>
@@ -2384,10 +2390,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:DT19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="CH1" activePane="topRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="CY19" sqref="CY19"/>
+      <selection pane="topRight" activeCell="DJ19" activeCellId="2" sqref="DF19 DI19 DJ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3007,7 +3013,7 @@
       <c r="BL16" s="11"/>
       <c r="BM16" s="11"/>
     </row>
-    <row r="17" spans="2:103" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:114" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>203</v>
       </c>
@@ -3016,14 +3022,14 @@
       <c r="AY17" s="11"/>
       <c r="AZ17" s="11"/>
     </row>
-    <row r="18" spans="2:103" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:114" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>213</v>
       </c>
       <c r="BO18" s="11"/>
       <c r="BP18" s="11"/>
     </row>
-    <row r="19" spans="2:103" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:114" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>229</v>
       </c>
@@ -3045,6 +3051,12 @@
       <c r="CU19" s="11"/>
       <c r="CW19" s="11"/>
       <c r="CY19" s="11"/>
+      <c r="DB19" s="11"/>
+      <c r="DC19" s="11"/>
+      <c r="DE19" s="11"/>
+      <c r="DF19" s="11"/>
+      <c r="DI19" s="11"/>
+      <c r="DJ19" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3145,10 +3157,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:CZ39"/>
+  <dimension ref="A3:DG39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="CN1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="CR1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -3186,10 +3198,15 @@
     <col min="98" max="98" width="20" customWidth="1"/>
     <col min="99" max="99" width="20.42578125" customWidth="1"/>
     <col min="101" max="101" width="14" customWidth="1"/>
+    <col min="105" max="105" width="11.140625" customWidth="1"/>
+    <col min="106" max="106" width="14.7109375" customWidth="1"/>
+    <col min="107" max="107" width="10.42578125" customWidth="1"/>
+    <col min="108" max="108" width="13.42578125" customWidth="1"/>
+    <col min="111" max="111" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:104" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:104" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:111" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:111" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>73</v>
       </c>
@@ -3427,8 +3444,27 @@
         <v>43623</v>
       </c>
       <c r="CZ4" s="54"/>
-    </row>
-    <row r="5" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="DA4" s="7">
+        <v>43626</v>
+      </c>
+      <c r="DB4" s="54">
+        <v>43627</v>
+      </c>
+      <c r="DC4" s="54"/>
+      <c r="DD4" s="7">
+        <v>43629</v>
+      </c>
+      <c r="DE4" s="7">
+        <v>43660</v>
+      </c>
+      <c r="DF4" s="7">
+        <v>43633</v>
+      </c>
+      <c r="DG4" s="7">
+        <v>43634</v>
+      </c>
+    </row>
+    <row r="5" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3450,7 +3486,7 @@
       <c r="BD5" s="40"/>
       <c r="BE5" s="40"/>
     </row>
-    <row r="6" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3464,7 +3500,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -3478,7 +3514,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -3492,7 +3528,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -3506,7 +3542,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -3516,7 +3552,7 @@
       <c r="C10" s="58"/>
       <c r="J10" s="61"/>
     </row>
-    <row r="11" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -3526,7 +3562,7 @@
       <c r="C11" s="59"/>
       <c r="J11" s="61"/>
     </row>
-    <row r="12" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -3540,7 +3576,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -3572,7 +3608,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -3607,7 +3643,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -3639,7 +3675,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3767,7 +3803,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -3796,7 +3832,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -3813,7 +3849,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -3821,7 +3857,7 @@
         <v>102</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="CA19" s="11" t="s">
         <v>216</v>
@@ -3901,8 +3937,29 @@
       <c r="CZ19" s="45" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="20" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="DA19" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="DB19" s="45" t="s">
+        <v>236</v>
+      </c>
+      <c r="DC19" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="DD19" s="45" t="s">
+        <v>230</v>
+      </c>
+      <c r="DE19" s="45" t="s">
+        <v>225</v>
+      </c>
+      <c r="DF19" s="45" t="s">
+        <v>237</v>
+      </c>
+      <c r="DG19" s="45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -3910,7 +3967,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -3918,7 +3975,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -3926,7 +3983,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -3934,7 +3991,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -3942,7 +3999,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -3950,7 +4007,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -3958,7 +4015,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -3966,15 +4023,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:104" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:111" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3983,9 +4040,10 @@
     <row r="38" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="CY4:CZ4"/>
-    <mergeCell ref="BL4:BM4"/>
+  <mergeCells count="30">
+    <mergeCell ref="CT4:CU4"/>
+    <mergeCell ref="CW4:CX4"/>
+    <mergeCell ref="CP4:CQ4"/>
     <mergeCell ref="BJ4:BK4"/>
     <mergeCell ref="BP4:BQ4"/>
     <mergeCell ref="C9:C11"/>
@@ -3997,9 +4055,10 @@
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="CT4:CU4"/>
-    <mergeCell ref="CW4:CX4"/>
-    <mergeCell ref="CP4:CQ4"/>
+    <mergeCell ref="CL4:CM4"/>
+    <mergeCell ref="CN4:CO4"/>
+    <mergeCell ref="AJ4:AM4"/>
+    <mergeCell ref="DB4:DC4"/>
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="BH4:BI4"/>
     <mergeCell ref="BE4:BG4"/>
@@ -4010,9 +4069,8 @@
     <mergeCell ref="AN4:AP4"/>
     <mergeCell ref="AQ4:AR4"/>
     <mergeCell ref="BB4:BC4"/>
-    <mergeCell ref="CL4:CM4"/>
-    <mergeCell ref="CN4:CO4"/>
-    <mergeCell ref="AJ4:AM4"/>
+    <mergeCell ref="CY4:CZ4"/>
+    <mergeCell ref="BL4:BM4"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:A27">
     <cfRule type="colorScale" priority="8">

</xml_diff>